<commit_message>
Correction on year 2006
</commit_message>
<xml_diff>
--- a/3_Backcasting analysis/analysis/Categorisation of risks/1. Summary of risks.xlsx
+++ b/3_Backcasting analysis/analysis/Categorisation of risks/1. Summary of risks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loudel30\.spyder-py3\WORK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41DEA83D-42D1-4675-95CF-D971AB7EF3CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{908D7C02-B78B-42B6-B6AF-85E37544C681}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{E553C518-F67A-44A5-955B-A68D03C7C977}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E553C518-F67A-44A5-955B-A68D03C7C977}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -2269,26 +2269,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC92BA55-D1EE-4422-A1E6-2482A068D892}">
   <dimension ref="A1:L533"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A291" zoomScale="95" workbookViewId="0">
-      <selection activeCell="I315" sqref="I315"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="95" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="62.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="70.7109375" customWidth="1"/>
+    <col min="2" max="2" width="62.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="70.6640625" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" customWidth="1"/>
-    <col min="6" max="6" width="19.140625" customWidth="1"/>
-    <col min="7" max="7" width="26.140625" customWidth="1"/>
-    <col min="8" max="8" width="29.85546875" customWidth="1"/>
-    <col min="9" max="9" width="16.7109375" customWidth="1"/>
-    <col min="10" max="10" width="19.140625" customWidth="1"/>
-    <col min="11" max="11" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" customWidth="1"/>
+    <col min="6" max="6" width="19.109375" customWidth="1"/>
+    <col min="7" max="7" width="26.109375" customWidth="1"/>
+    <col min="8" max="8" width="29.88671875" customWidth="1"/>
+    <col min="9" max="9" width="16.6640625" customWidth="1"/>
+    <col min="10" max="10" width="19.109375" customWidth="1"/>
+    <col min="11" max="11" width="27.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2326,7 +2326,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2006</v>
       </c>
@@ -2348,7 +2348,7 @@
       <c r="K2" s="5"/>
       <c r="L2" s="5"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2006</v>
       </c>
@@ -2368,7 +2368,7 @@
       <c r="K3" s="4"/>
       <c r="L3" s="4"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2006</v>
       </c>
@@ -2388,7 +2388,7 @@
       <c r="K4" s="4"/>
       <c r="L4" s="4"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2006</v>
       </c>
@@ -2410,7 +2410,7 @@
       <c r="K5" s="4"/>
       <c r="L5" s="4"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2006</v>
       </c>
@@ -2432,7 +2432,7 @@
       <c r="K6" s="4"/>
       <c r="L6" s="4"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2006</v>
       </c>
@@ -2454,7 +2454,7 @@
       <c r="K7" s="4"/>
       <c r="L7" s="4"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2006</v>
       </c>
@@ -2474,7 +2474,7 @@
       <c r="K8" s="4"/>
       <c r="L8" s="4"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2006</v>
       </c>
@@ -2494,7 +2494,7 @@
       <c r="K9" s="4"/>
       <c r="L9" s="4"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2006</v>
       </c>
@@ -2505,12 +2505,8 @@
       <c r="D10" s="4">
         <v>1.5</v>
       </c>
-      <c r="E10" s="4">
-        <v>1</v>
-      </c>
-      <c r="F10" s="4">
-        <v>1</v>
-      </c>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
@@ -2518,7 +2514,7 @@
       <c r="K10" s="4"/>
       <c r="L10" s="4"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2006</v>
       </c>
@@ -2529,12 +2525,8 @@
       <c r="D11" s="4">
         <v>1.5</v>
       </c>
-      <c r="E11" s="4">
-        <v>1</v>
-      </c>
-      <c r="F11" s="4">
-        <v>1</v>
-      </c>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
@@ -2542,7 +2534,7 @@
       <c r="K11" s="4"/>
       <c r="L11" s="4"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>2006</v>
       </c>
@@ -2564,7 +2556,7 @@
       <c r="K12" s="4"/>
       <c r="L12" s="4"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>2006</v>
       </c>
@@ -2588,7 +2580,7 @@
       <c r="K13" s="4"/>
       <c r="L13" s="4"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2006</v>
       </c>
@@ -2608,7 +2600,7 @@
       <c r="K14" s="4"/>
       <c r="L14" s="4"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2006</v>
       </c>
@@ -2628,7 +2620,7 @@
       <c r="K15" s="4"/>
       <c r="L15" s="4"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2006</v>
       </c>
@@ -2648,7 +2640,7 @@
       <c r="K16" s="4"/>
       <c r="L16" s="4"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>2006</v>
       </c>
@@ -2668,7 +2660,7 @@
       <c r="K17" s="4"/>
       <c r="L17" s="4"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>2006</v>
       </c>
@@ -2688,7 +2680,7 @@
       <c r="K18" s="4"/>
       <c r="L18" s="4"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>2006</v>
       </c>
@@ -2708,7 +2700,7 @@
       <c r="K19" s="4"/>
       <c r="L19" s="4"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>2006</v>
       </c>
@@ -2728,7 +2720,7 @@
       <c r="K20" s="4"/>
       <c r="L20" s="4"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>2006</v>
       </c>
@@ -2750,7 +2742,7 @@
       </c>
       <c r="L21" s="4"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>2006</v>
       </c>
@@ -2770,7 +2762,7 @@
       <c r="K22" s="4"/>
       <c r="L22" s="4"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>2006</v>
       </c>
@@ -2790,7 +2782,7 @@
       <c r="K23" s="4"/>
       <c r="L23" s="4"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>2006</v>
       </c>
@@ -2810,7 +2802,7 @@
       <c r="K24" s="4"/>
       <c r="L24" s="4"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>2006</v>
       </c>
@@ -2830,7 +2822,7 @@
       <c r="K25" s="4"/>
       <c r="L25" s="4"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>2006</v>
       </c>
@@ -2852,7 +2844,7 @@
       <c r="K26" s="4"/>
       <c r="L26" s="4"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>2006</v>
       </c>
@@ -2874,7 +2866,7 @@
       <c r="K27" s="4"/>
       <c r="L27" s="4"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>2006</v>
       </c>
@@ -2894,7 +2886,7 @@
       <c r="K28" s="4"/>
       <c r="L28" s="4"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>2006</v>
       </c>
@@ -2914,7 +2906,7 @@
       <c r="K29" s="4"/>
       <c r="L29" s="4"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>2006</v>
       </c>
@@ -2934,7 +2926,7 @@
       <c r="K30" s="4"/>
       <c r="L30" s="4"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>2006</v>
       </c>
@@ -2954,7 +2946,7 @@
       <c r="K31" s="4"/>
       <c r="L31" s="4"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>2006</v>
       </c>
@@ -2974,7 +2966,7 @@
       <c r="K32" s="4"/>
       <c r="L32" s="4"/>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>2007</v>
       </c>
@@ -2996,7 +2988,7 @@
       <c r="K33" s="4"/>
       <c r="L33" s="4"/>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>2007</v>
       </c>
@@ -3016,7 +3008,7 @@
       <c r="K34" s="4"/>
       <c r="L34" s="4"/>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>2007</v>
       </c>
@@ -3036,7 +3028,7 @@
       <c r="K35" s="4"/>
       <c r="L35" s="4"/>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>2007</v>
       </c>
@@ -3058,7 +3050,7 @@
       <c r="K36" s="4"/>
       <c r="L36" s="4"/>
     </row>
-    <row r="37" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>2007</v>
       </c>
@@ -3080,7 +3072,7 @@
       <c r="K37" s="4"/>
       <c r="L37" s="4"/>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>2007</v>
       </c>
@@ -3102,7 +3094,7 @@
       <c r="K38" s="4"/>
       <c r="L38" s="4"/>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>2007</v>
       </c>
@@ -3124,7 +3116,7 @@
       <c r="K39" s="4"/>
       <c r="L39" s="4"/>
     </row>
-    <row r="40" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>2007</v>
       </c>
@@ -3144,7 +3136,7 @@
       <c r="K40" s="4"/>
       <c r="L40" s="4"/>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>2007</v>
       </c>
@@ -3166,7 +3158,7 @@
       <c r="K41" s="4"/>
       <c r="L41" s="4"/>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>2007</v>
       </c>
@@ -3186,7 +3178,7 @@
       <c r="K42" s="4"/>
       <c r="L42" s="4"/>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>2007</v>
       </c>
@@ -3208,7 +3200,7 @@
       </c>
       <c r="L43" s="4"/>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>2007</v>
       </c>
@@ -3228,7 +3220,7 @@
       <c r="K44" s="4"/>
       <c r="L44" s="4"/>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>2007</v>
       </c>
@@ -3250,7 +3242,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>2007</v>
       </c>
@@ -3272,7 +3264,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>2007</v>
       </c>
@@ -3292,7 +3284,7 @@
       <c r="K47" s="4"/>
       <c r="L47" s="4"/>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>2007</v>
       </c>
@@ -3312,7 +3304,7 @@
       <c r="K48" s="4"/>
       <c r="L48" s="4"/>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>2007</v>
       </c>
@@ -3332,7 +3324,7 @@
       <c r="K49" s="4"/>
       <c r="L49" s="4"/>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>2007</v>
       </c>
@@ -3354,7 +3346,7 @@
       <c r="K50" s="4"/>
       <c r="L50" s="4"/>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>2007</v>
       </c>
@@ -3376,7 +3368,7 @@
       <c r="K51" s="4"/>
       <c r="L51" s="4"/>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>2007</v>
       </c>
@@ -3396,7 +3388,7 @@
       <c r="K52" s="4"/>
       <c r="L52" s="4"/>
     </row>
-    <row r="53" spans="1:12" ht="36" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" ht="36" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>2007</v>
       </c>
@@ -3418,7 +3410,7 @@
       <c r="K53" s="4"/>
       <c r="L53" s="4"/>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>2007</v>
       </c>
@@ -3440,7 +3432,7 @@
       <c r="K54" s="4"/>
       <c r="L54" s="4"/>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>2007</v>
       </c>
@@ -3460,7 +3452,7 @@
       <c r="K55" s="4"/>
       <c r="L55" s="4"/>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>2008</v>
       </c>
@@ -3480,7 +3472,7 @@
       <c r="K56" s="4"/>
       <c r="L56" s="4"/>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>2008</v>
       </c>
@@ -3502,7 +3494,7 @@
       <c r="K57" s="4"/>
       <c r="L57" s="4"/>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>2008</v>
       </c>
@@ -3522,7 +3514,7 @@
       <c r="K58" s="4"/>
       <c r="L58" s="4"/>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>2008</v>
       </c>
@@ -3542,7 +3534,7 @@
       <c r="K59" s="4"/>
       <c r="L59" s="4"/>
     </row>
-    <row r="60" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>2008</v>
       </c>
@@ -3566,7 +3558,7 @@
       <c r="K60" s="4"/>
       <c r="L60" s="4"/>
     </row>
-    <row r="61" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>2008</v>
       </c>
@@ -3590,7 +3582,7 @@
       <c r="K61" s="4"/>
       <c r="L61" s="4"/>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>2008</v>
       </c>
@@ -3612,7 +3604,7 @@
       <c r="K62" s="4"/>
       <c r="L62" s="4"/>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>2008</v>
       </c>
@@ -3632,7 +3624,7 @@
       <c r="K63" s="4"/>
       <c r="L63" s="4"/>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>2008</v>
       </c>
@@ -3654,7 +3646,7 @@
       <c r="K64" s="4"/>
       <c r="L64" s="4"/>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>2008</v>
       </c>
@@ -3674,7 +3666,7 @@
       <c r="K65" s="4"/>
       <c r="L65" s="4"/>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>2008</v>
       </c>
@@ -3696,7 +3688,7 @@
       <c r="K66" s="4"/>
       <c r="L66" s="4"/>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>2008</v>
       </c>
@@ -3716,7 +3708,7 @@
       <c r="K67" s="4"/>
       <c r="L67" s="4"/>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>2008</v>
       </c>
@@ -3738,7 +3730,7 @@
       </c>
       <c r="L68" s="4"/>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>2008</v>
       </c>
@@ -3758,7 +3750,7 @@
       <c r="K69" s="4"/>
       <c r="L69" s="4"/>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>2008</v>
       </c>
@@ -3780,7 +3772,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>2008</v>
       </c>
@@ -3800,7 +3792,7 @@
       <c r="K71" s="4"/>
       <c r="L71" s="4"/>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>2008</v>
       </c>
@@ -3820,7 +3812,7 @@
       <c r="K72" s="4"/>
       <c r="L72" s="4"/>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>2008</v>
       </c>
@@ -3840,7 +3832,7 @@
       <c r="K73" s="4"/>
       <c r="L73" s="4"/>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>2008</v>
       </c>
@@ -3860,7 +3852,7 @@
       <c r="K74" s="4"/>
       <c r="L74" s="4"/>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>2008</v>
       </c>
@@ -3882,7 +3874,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>2008</v>
       </c>
@@ -3904,7 +3896,7 @@
       <c r="K76" s="4"/>
       <c r="L76" s="4"/>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>2008</v>
       </c>
@@ -3926,7 +3918,7 @@
       <c r="K77" s="4"/>
       <c r="L77" s="4"/>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>2008</v>
       </c>
@@ -3946,7 +3938,7 @@
       <c r="K78" s="4"/>
       <c r="L78" s="4"/>
     </row>
-    <row r="79" spans="1:12" ht="36" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:12" ht="36" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>2008</v>
       </c>
@@ -3968,7 +3960,7 @@
       <c r="K79" s="4"/>
       <c r="L79" s="4"/>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>2008</v>
       </c>
@@ -3990,7 +3982,7 @@
       <c r="K80" s="4"/>
       <c r="L80" s="4"/>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>2008</v>
       </c>
@@ -4010,7 +4002,7 @@
       <c r="K81" s="4"/>
       <c r="L81" s="4"/>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>2009</v>
       </c>
@@ -4032,7 +4024,7 @@
       <c r="K82" s="4"/>
       <c r="L82" s="4"/>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>2009</v>
       </c>
@@ -4054,7 +4046,7 @@
       <c r="K83" s="4"/>
       <c r="L83" s="4"/>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>2009</v>
       </c>
@@ -4074,7 +4066,7 @@
       <c r="K84" s="4"/>
       <c r="L84" s="4"/>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>2009</v>
       </c>
@@ -4094,7 +4086,7 @@
       <c r="K85" s="4"/>
       <c r="L85" s="4"/>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>2009</v>
       </c>
@@ -4116,7 +4108,7 @@
       <c r="K86" s="4"/>
       <c r="L86" s="4"/>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>2009</v>
       </c>
@@ -4138,7 +4130,7 @@
       <c r="K87" s="4"/>
       <c r="L87" s="4"/>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>2009</v>
       </c>
@@ -4158,7 +4150,7 @@
       <c r="K88" s="4"/>
       <c r="L88" s="4"/>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>2009</v>
       </c>
@@ -4178,7 +4170,7 @@
       <c r="K89" s="4"/>
       <c r="L89" s="4"/>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>2009</v>
       </c>
@@ -4198,7 +4190,7 @@
       <c r="K90" s="4"/>
       <c r="L90" s="4"/>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>2009</v>
       </c>
@@ -4220,7 +4212,7 @@
       <c r="K91" s="4"/>
       <c r="L91" s="4"/>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>2009</v>
       </c>
@@ -4242,7 +4234,7 @@
       <c r="K92" s="4"/>
       <c r="L92" s="4"/>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>2009</v>
       </c>
@@ -4264,7 +4256,7 @@
       <c r="K93" s="4"/>
       <c r="L93" s="4"/>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>2009</v>
       </c>
@@ -4284,7 +4276,7 @@
       <c r="K94" s="4"/>
       <c r="L94" s="4"/>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>2009</v>
       </c>
@@ -4306,7 +4298,7 @@
       <c r="K95" s="4"/>
       <c r="L95" s="4"/>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>2009</v>
       </c>
@@ -4326,7 +4318,7 @@
       <c r="K96" s="4"/>
       <c r="L96" s="4"/>
     </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>2009</v>
       </c>
@@ -4348,7 +4340,7 @@
       <c r="K97" s="4"/>
       <c r="L97" s="4"/>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>2009</v>
       </c>
@@ -4368,7 +4360,7 @@
       <c r="K98" s="4"/>
       <c r="L98" s="4"/>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>2009</v>
       </c>
@@ -4388,7 +4380,7 @@
       <c r="K99" s="4"/>
       <c r="L99" s="4"/>
     </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>2009</v>
       </c>
@@ -4408,7 +4400,7 @@
       <c r="K100" s="4"/>
       <c r="L100" s="4"/>
     </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>2009</v>
       </c>
@@ -4430,7 +4422,7 @@
       </c>
       <c r="L101" s="4"/>
     </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>2009</v>
       </c>
@@ -4450,7 +4442,7 @@
       <c r="K102" s="4"/>
       <c r="L102" s="4"/>
     </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>2009</v>
       </c>
@@ -4470,7 +4462,7 @@
       <c r="K103" s="4"/>
       <c r="L103" s="4"/>
     </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>2009</v>
       </c>
@@ -4490,7 +4482,7 @@
       <c r="K104" s="4"/>
       <c r="L104" s="4"/>
     </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>2009</v>
       </c>
@@ -4510,7 +4502,7 @@
       <c r="K105" s="4"/>
       <c r="L105" s="4"/>
     </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>2009</v>
       </c>
@@ -4530,7 +4522,7 @@
       <c r="K106" s="4"/>
       <c r="L106" s="4"/>
     </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>2009</v>
       </c>
@@ -4550,7 +4542,7 @@
       <c r="K107" s="4"/>
       <c r="L107" s="4"/>
     </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>2009</v>
       </c>
@@ -4570,7 +4562,7 @@
       <c r="K108" s="4"/>
       <c r="L108" s="4"/>
     </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>2009</v>
       </c>
@@ -4590,7 +4582,7 @@
       <c r="K109" s="4"/>
       <c r="L109" s="4"/>
     </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>2009</v>
       </c>
@@ -4612,7 +4604,7 @@
       <c r="K110" s="4"/>
       <c r="L110" s="4"/>
     </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>2009</v>
       </c>
@@ -4634,7 +4626,7 @@
       <c r="K111" s="4"/>
       <c r="L111" s="4"/>
     </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>2009</v>
       </c>
@@ -4654,7 +4646,7 @@
       <c r="K112" s="4"/>
       <c r="L112" s="4"/>
     </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>2009</v>
       </c>
@@ -4674,7 +4666,7 @@
       <c r="K113" s="4"/>
       <c r="L113" s="4"/>
     </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>2009</v>
       </c>
@@ -4694,7 +4686,7 @@
       <c r="K114" s="4"/>
       <c r="L114" s="4"/>
     </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>2009</v>
       </c>
@@ -4716,7 +4708,7 @@
       <c r="K115" s="4"/>
       <c r="L115" s="4"/>
     </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>2009</v>
       </c>
@@ -4736,7 +4728,7 @@
       <c r="K116" s="4"/>
       <c r="L116" s="4"/>
     </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>2009</v>
       </c>
@@ -4756,7 +4748,7 @@
       <c r="K117" s="4"/>
       <c r="L117" s="4"/>
     </row>
-    <row r="118" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>2010</v>
       </c>
@@ -4780,7 +4772,7 @@
       <c r="K118" s="4"/>
       <c r="L118" s="4"/>
     </row>
-    <row r="119" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>2010</v>
       </c>
@@ -4804,7 +4796,7 @@
       <c r="K119" s="4"/>
       <c r="L119" s="4"/>
     </row>
-    <row r="120" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>2010</v>
       </c>
@@ -4826,7 +4818,7 @@
       <c r="K120" s="4"/>
       <c r="L120" s="4"/>
     </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>2010</v>
       </c>
@@ -4848,7 +4840,7 @@
       <c r="K121" s="4"/>
       <c r="L121" s="4"/>
     </row>
-    <row r="122" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>2010</v>
       </c>
@@ -4872,7 +4864,7 @@
       <c r="K122" s="4"/>
       <c r="L122" s="4"/>
     </row>
-    <row r="123" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>2010</v>
       </c>
@@ -4896,7 +4888,7 @@
       <c r="K123" s="4"/>
       <c r="L123" s="4"/>
     </row>
-    <row r="124" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>2010</v>
       </c>
@@ -4918,7 +4910,7 @@
       <c r="K124" s="4"/>
       <c r="L124" s="4"/>
     </row>
-    <row r="125" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>2010</v>
       </c>
@@ -4940,7 +4932,7 @@
       <c r="K125" s="4"/>
       <c r="L125" s="4"/>
     </row>
-    <row r="126" spans="1:12" ht="36" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:12" ht="36" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>2010</v>
       </c>
@@ -4962,7 +4954,7 @@
       <c r="K126" s="4"/>
       <c r="L126" s="4"/>
     </row>
-    <row r="127" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>2010</v>
       </c>
@@ -4986,7 +4978,7 @@
       <c r="K127" s="4"/>
       <c r="L127" s="4"/>
     </row>
-    <row r="128" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>2010</v>
       </c>
@@ -5010,7 +5002,7 @@
       <c r="K128" s="4"/>
       <c r="L128" s="4"/>
     </row>
-    <row r="129" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>2010</v>
       </c>
@@ -5032,7 +5024,7 @@
       <c r="K129" s="4"/>
       <c r="L129" s="4"/>
     </row>
-    <row r="130" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>2010</v>
       </c>
@@ -5056,7 +5048,7 @@
       <c r="K130" s="4"/>
       <c r="L130" s="4"/>
     </row>
-    <row r="131" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>2010</v>
       </c>
@@ -5078,7 +5070,7 @@
       <c r="K131" s="4"/>
       <c r="L131" s="4"/>
     </row>
-    <row r="132" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>2010</v>
       </c>
@@ -5102,7 +5094,7 @@
       <c r="K132" s="4"/>
       <c r="L132" s="4"/>
     </row>
-    <row r="133" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>2010</v>
       </c>
@@ -5124,7 +5116,7 @@
       <c r="K133" s="4"/>
       <c r="L133" s="4"/>
     </row>
-    <row r="134" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>2010</v>
       </c>
@@ -5146,7 +5138,7 @@
       <c r="K134" s="4"/>
       <c r="L134" s="4"/>
     </row>
-    <row r="135" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>2010</v>
       </c>
@@ -5168,7 +5160,7 @@
       <c r="K135" s="4"/>
       <c r="L135" s="4"/>
     </row>
-    <row r="136" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>2010</v>
       </c>
@@ -5192,7 +5184,7 @@
       <c r="K136" s="4"/>
       <c r="L136" s="4"/>
     </row>
-    <row r="137" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>2010</v>
       </c>
@@ -5216,7 +5208,7 @@
       </c>
       <c r="L137" s="4"/>
     </row>
-    <row r="138" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>2010</v>
       </c>
@@ -5238,7 +5230,7 @@
       <c r="K138" s="4"/>
       <c r="L138" s="4"/>
     </row>
-    <row r="139" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>2010</v>
       </c>
@@ -5260,7 +5252,7 @@
       <c r="K139" s="4"/>
       <c r="L139" s="4"/>
     </row>
-    <row r="140" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>2010</v>
       </c>
@@ -5282,7 +5274,7 @@
       <c r="K140" s="4"/>
       <c r="L140" s="4"/>
     </row>
-    <row r="141" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>2010</v>
       </c>
@@ -5304,7 +5296,7 @@
       <c r="K141" s="4"/>
       <c r="L141" s="4"/>
     </row>
-    <row r="142" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>2010</v>
       </c>
@@ -5326,7 +5318,7 @@
       <c r="K142" s="4"/>
       <c r="L142" s="4"/>
     </row>
-    <row r="143" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>2010</v>
       </c>
@@ -5348,7 +5340,7 @@
       <c r="K143" s="4"/>
       <c r="L143" s="4"/>
     </row>
-    <row r="144" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>2010</v>
       </c>
@@ -5370,7 +5362,7 @@
       <c r="K144" s="4"/>
       <c r="L144" s="4"/>
     </row>
-    <row r="145" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A145">
         <v>2010</v>
       </c>
@@ -5392,7 +5384,7 @@
       <c r="K145" s="4"/>
       <c r="L145" s="4"/>
     </row>
-    <row r="146" spans="1:12" ht="36" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:12" ht="36" x14ac:dyDescent="0.3">
       <c r="A146">
         <v>2010</v>
       </c>
@@ -5416,7 +5408,7 @@
       <c r="K146" s="4"/>
       <c r="L146" s="4"/>
     </row>
-    <row r="147" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A147">
         <v>2010</v>
       </c>
@@ -5440,7 +5432,7 @@
       <c r="K147" s="4"/>
       <c r="L147" s="4"/>
     </row>
-    <row r="148" spans="1:12" ht="36" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:12" ht="36" x14ac:dyDescent="0.3">
       <c r="A148">
         <v>2010</v>
       </c>
@@ -5462,7 +5454,7 @@
       <c r="K148" s="4"/>
       <c r="L148" s="4"/>
     </row>
-    <row r="149" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A149">
         <v>2010</v>
       </c>
@@ -5484,7 +5476,7 @@
       <c r="K149" s="4"/>
       <c r="L149" s="4"/>
     </row>
-    <row r="150" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A150">
         <v>2010</v>
       </c>
@@ -5506,7 +5498,7 @@
       <c r="K150" s="4"/>
       <c r="L150" s="4"/>
     </row>
-    <row r="151" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A151">
         <v>2010</v>
       </c>
@@ -5530,7 +5522,7 @@
       <c r="K151" s="4"/>
       <c r="L151" s="4"/>
     </row>
-    <row r="152" spans="1:12" ht="36" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:12" ht="36" x14ac:dyDescent="0.3">
       <c r="A152">
         <v>2010</v>
       </c>
@@ -5552,7 +5544,7 @@
       <c r="K152" s="4"/>
       <c r="L152" s="4"/>
     </row>
-    <row r="153" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A153">
         <v>2010</v>
       </c>
@@ -5574,7 +5566,7 @@
       <c r="K153" s="4"/>
       <c r="L153" s="4"/>
     </row>
-    <row r="154" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A154">
         <v>2011</v>
       </c>
@@ -5596,7 +5588,7 @@
       <c r="K154" s="4"/>
       <c r="L154" s="4"/>
     </row>
-    <row r="155" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A155">
         <v>2011</v>
       </c>
@@ -5616,7 +5608,7 @@
       <c r="K155" s="4"/>
       <c r="L155" s="4"/>
     </row>
-    <row r="156" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A156">
         <v>2011</v>
       </c>
@@ -5638,7 +5630,7 @@
       <c r="K156" s="4"/>
       <c r="L156" s="4"/>
     </row>
-    <row r="157" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A157">
         <v>2011</v>
       </c>
@@ -5660,7 +5652,7 @@
       <c r="K157" s="4"/>
       <c r="L157" s="4"/>
     </row>
-    <row r="158" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A158">
         <v>2011</v>
       </c>
@@ -5682,7 +5674,7 @@
       <c r="K158" s="4"/>
       <c r="L158" s="4"/>
     </row>
-    <row r="159" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A159">
         <v>2011</v>
       </c>
@@ -5702,7 +5694,7 @@
       <c r="K159" s="4"/>
       <c r="L159" s="4"/>
     </row>
-    <row r="160" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A160">
         <v>2011</v>
       </c>
@@ -5722,7 +5714,7 @@
       <c r="K160" s="4"/>
       <c r="L160" s="4"/>
     </row>
-    <row r="161" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A161">
         <v>2011</v>
       </c>
@@ -5742,7 +5734,7 @@
       <c r="K161" s="4"/>
       <c r="L161" s="4"/>
     </row>
-    <row r="162" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A162">
         <v>2011</v>
       </c>
@@ -5764,7 +5756,7 @@
       <c r="K162" s="4"/>
       <c r="L162" s="4"/>
     </row>
-    <row r="163" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A163">
         <v>2011</v>
       </c>
@@ -5784,7 +5776,7 @@
       <c r="K163" s="4"/>
       <c r="L163" s="4"/>
     </row>
-    <row r="164" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A164">
         <v>2011</v>
       </c>
@@ -5806,7 +5798,7 @@
       <c r="K164" s="4"/>
       <c r="L164" s="4"/>
     </row>
-    <row r="165" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A165">
         <v>2011</v>
       </c>
@@ -5826,7 +5818,7 @@
       <c r="K165" s="4"/>
       <c r="L165" s="4"/>
     </row>
-    <row r="166" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A166">
         <v>2011</v>
       </c>
@@ -5848,7 +5840,7 @@
       <c r="K166" s="4"/>
       <c r="L166" s="4"/>
     </row>
-    <row r="167" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A167">
         <v>2011</v>
       </c>
@@ -5870,7 +5862,7 @@
       <c r="K167" s="4"/>
       <c r="L167" s="4"/>
     </row>
-    <row r="168" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A168">
         <v>2011</v>
       </c>
@@ -5892,7 +5884,7 @@
       <c r="K168" s="4"/>
       <c r="L168" s="4"/>
     </row>
-    <row r="169" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A169">
         <v>2011</v>
       </c>
@@ -5912,7 +5904,7 @@
       <c r="K169" s="4"/>
       <c r="L169" s="4"/>
     </row>
-    <row r="170" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A170">
         <v>2011</v>
       </c>
@@ -5932,7 +5924,7 @@
       <c r="K170" s="4"/>
       <c r="L170" s="4"/>
     </row>
-    <row r="171" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A171">
         <v>2011</v>
       </c>
@@ -5952,7 +5944,7 @@
       <c r="K171" s="4"/>
       <c r="L171" s="4"/>
     </row>
-    <row r="172" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A172">
         <v>2011</v>
       </c>
@@ -5972,7 +5964,7 @@
       <c r="K172" s="4"/>
       <c r="L172" s="4"/>
     </row>
-    <row r="173" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A173">
         <v>2011</v>
       </c>
@@ -5994,7 +5986,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="174" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A174">
         <v>2011</v>
       </c>
@@ -6016,7 +6008,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="175" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A175">
         <v>2011</v>
       </c>
@@ -6036,7 +6028,7 @@
       <c r="K175" s="4"/>
       <c r="L175" s="4"/>
     </row>
-    <row r="176" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A176">
         <v>2011</v>
       </c>
@@ -6056,7 +6048,7 @@
       <c r="K176" s="4"/>
       <c r="L176" s="4"/>
     </row>
-    <row r="177" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A177">
         <v>2011</v>
       </c>
@@ -6076,7 +6068,7 @@
       <c r="K177" s="4"/>
       <c r="L177" s="4"/>
     </row>
-    <row r="178" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A178">
         <v>2011</v>
       </c>
@@ -6098,7 +6090,7 @@
       </c>
       <c r="L178" s="4"/>
     </row>
-    <row r="179" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A179">
         <v>2011</v>
       </c>
@@ -6118,7 +6110,7 @@
       <c r="K179" s="4"/>
       <c r="L179" s="4"/>
     </row>
-    <row r="180" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A180">
         <v>2011</v>
       </c>
@@ -6138,7 +6130,7 @@
       <c r="K180" s="4"/>
       <c r="L180" s="4"/>
     </row>
-    <row r="181" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A181">
         <v>2011</v>
       </c>
@@ -6158,7 +6150,7 @@
       <c r="K181" s="4"/>
       <c r="L181" s="4"/>
     </row>
-    <row r="182" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A182">
         <v>2011</v>
       </c>
@@ -6180,7 +6172,7 @@
       <c r="K182" s="4"/>
       <c r="L182" s="4"/>
     </row>
-    <row r="183" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A183">
         <v>2011</v>
       </c>
@@ -6202,7 +6194,7 @@
       <c r="K183" s="4"/>
       <c r="L183" s="4"/>
     </row>
-    <row r="184" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A184">
         <v>2011</v>
       </c>
@@ -6222,7 +6214,7 @@
       <c r="K184" s="4"/>
       <c r="L184" s="4"/>
     </row>
-    <row r="185" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A185">
         <v>2011</v>
       </c>
@@ -6242,7 +6234,7 @@
       <c r="K185" s="4"/>
       <c r="L185" s="4"/>
     </row>
-    <row r="186" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A186">
         <v>2011</v>
       </c>
@@ -6264,7 +6256,7 @@
       <c r="K186" s="4"/>
       <c r="L186" s="4"/>
     </row>
-    <row r="187" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A187">
         <v>2011</v>
       </c>
@@ -6284,7 +6276,7 @@
       <c r="K187" s="4"/>
       <c r="L187" s="4"/>
     </row>
-    <row r="188" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A188">
         <v>2011</v>
       </c>
@@ -6306,7 +6298,7 @@
       <c r="K188" s="4"/>
       <c r="L188" s="4"/>
     </row>
-    <row r="189" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A189">
         <v>2011</v>
       </c>
@@ -6326,7 +6318,7 @@
       <c r="K189" s="4"/>
       <c r="L189" s="4"/>
     </row>
-    <row r="190" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A190">
         <v>2011</v>
       </c>
@@ -6346,7 +6338,7 @@
       <c r="K190" s="4"/>
       <c r="L190" s="4"/>
     </row>
-    <row r="191" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A191">
         <v>2012</v>
       </c>
@@ -6370,7 +6362,7 @@
       <c r="K191" s="4"/>
       <c r="L191" s="4"/>
     </row>
-    <row r="192" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A192">
         <v>2012</v>
       </c>
@@ -6392,7 +6384,7 @@
       <c r="K192" s="4"/>
       <c r="L192" s="4"/>
     </row>
-    <row r="193" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A193">
         <v>2012</v>
       </c>
@@ -6416,7 +6408,7 @@
       <c r="K193" s="4"/>
       <c r="L193" s="4"/>
     </row>
-    <row r="194" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A194">
         <v>2012</v>
       </c>
@@ -6438,7 +6430,7 @@
       <c r="K194" s="4"/>
       <c r="L194" s="4"/>
     </row>
-    <row r="195" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A195">
         <v>2012</v>
       </c>
@@ -6462,7 +6454,7 @@
       <c r="K195" s="4"/>
       <c r="L195" s="4"/>
     </row>
-    <row r="196" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A196">
         <v>2012</v>
       </c>
@@ -6486,7 +6478,7 @@
       <c r="K196" s="4"/>
       <c r="L196" s="4"/>
     </row>
-    <row r="197" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A197">
         <v>2012</v>
       </c>
@@ -6510,7 +6502,7 @@
       <c r="K197" s="4"/>
       <c r="L197" s="4"/>
     </row>
-    <row r="198" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A198">
         <v>2012</v>
       </c>
@@ -6532,7 +6524,7 @@
       <c r="K198" s="4"/>
       <c r="L198" s="4"/>
     </row>
-    <row r="199" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A199">
         <v>2012</v>
       </c>
@@ -6554,7 +6546,7 @@
       <c r="K199" s="4"/>
       <c r="L199" s="4"/>
     </row>
-    <row r="200" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A200">
         <v>2012</v>
       </c>
@@ -6576,7 +6568,7 @@
       <c r="K200" s="4"/>
       <c r="L200" s="4"/>
     </row>
-    <row r="201" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A201">
         <v>2012</v>
       </c>
@@ -6598,7 +6590,7 @@
       <c r="K201" s="4"/>
       <c r="L201" s="4"/>
     </row>
-    <row r="202" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A202">
         <v>2012</v>
       </c>
@@ -6620,7 +6612,7 @@
       <c r="K202" s="4"/>
       <c r="L202" s="4"/>
     </row>
-    <row r="203" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A203">
         <v>2012</v>
       </c>
@@ -6644,7 +6636,7 @@
       <c r="K203" s="4"/>
       <c r="L203" s="4"/>
     </row>
-    <row r="204" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A204">
         <v>2012</v>
       </c>
@@ -6668,7 +6660,7 @@
       <c r="K204" s="4"/>
       <c r="L204" s="4"/>
     </row>
-    <row r="205" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A205">
         <v>2012</v>
       </c>
@@ -6690,7 +6682,7 @@
       <c r="K205" s="4"/>
       <c r="L205" s="4"/>
     </row>
-    <row r="206" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A206">
         <v>2012</v>
       </c>
@@ -6714,7 +6706,7 @@
       <c r="K206" s="4"/>
       <c r="L206" s="4"/>
     </row>
-    <row r="207" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A207">
         <v>2012</v>
       </c>
@@ -6736,7 +6728,7 @@
       <c r="K207" s="4"/>
       <c r="L207" s="4"/>
     </row>
-    <row r="208" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A208">
         <v>2012</v>
       </c>
@@ -6760,7 +6752,7 @@
       <c r="K208" s="4"/>
       <c r="L208" s="4"/>
     </row>
-    <row r="209" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A209">
         <v>2012</v>
       </c>
@@ -6784,7 +6776,7 @@
       <c r="K209" s="4"/>
       <c r="L209" s="4"/>
     </row>
-    <row r="210" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A210">
         <v>2012</v>
       </c>
@@ -6806,7 +6798,7 @@
       <c r="K210" s="4"/>
       <c r="L210" s="4"/>
     </row>
-    <row r="211" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A211">
         <v>2012</v>
       </c>
@@ -6830,7 +6822,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="212" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A212">
         <v>2012</v>
       </c>
@@ -6852,7 +6844,7 @@
       <c r="K212" s="4"/>
       <c r="L212" s="4"/>
     </row>
-    <row r="213" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A213">
         <v>2012</v>
       </c>
@@ -6874,7 +6866,7 @@
       <c r="K213" s="4"/>
       <c r="L213" s="4"/>
     </row>
-    <row r="214" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A214">
         <v>2012</v>
       </c>
@@ -6898,7 +6890,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="215" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A215">
         <v>2012</v>
       </c>
@@ -6920,7 +6912,7 @@
       <c r="K215" s="4"/>
       <c r="L215" s="4"/>
     </row>
-    <row r="216" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A216">
         <v>2012</v>
       </c>
@@ -6942,7 +6934,7 @@
       <c r="K216" s="4"/>
       <c r="L216" s="4"/>
     </row>
-    <row r="217" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A217">
         <v>2012</v>
       </c>
@@ -6966,7 +6958,7 @@
       </c>
       <c r="L217" s="4"/>
     </row>
-    <row r="218" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A218">
         <v>2012</v>
       </c>
@@ -6988,7 +6980,7 @@
       <c r="K218" s="4"/>
       <c r="L218" s="4"/>
     </row>
-    <row r="219" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A219">
         <v>2012</v>
       </c>
@@ -7010,7 +7002,7 @@
       <c r="K219" s="4"/>
       <c r="L219" s="4"/>
     </row>
-    <row r="220" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A220">
         <v>2012</v>
       </c>
@@ -7032,7 +7024,7 @@
       <c r="K220" s="4"/>
       <c r="L220" s="4"/>
     </row>
-    <row r="221" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A221">
         <v>2012</v>
       </c>
@@ -7054,7 +7046,7 @@
       <c r="K221" s="4"/>
       <c r="L221" s="4"/>
     </row>
-    <row r="222" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A222">
         <v>2012</v>
       </c>
@@ -7078,7 +7070,7 @@
       <c r="K222" s="4"/>
       <c r="L222" s="4"/>
     </row>
-    <row r="223" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A223">
         <v>2012</v>
       </c>
@@ -7100,7 +7092,7 @@
       <c r="K223" s="4"/>
       <c r="L223" s="4"/>
     </row>
-    <row r="224" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A224">
         <v>2012</v>
       </c>
@@ -7122,7 +7114,7 @@
       <c r="K224" s="4"/>
       <c r="L224" s="4"/>
     </row>
-    <row r="225" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A225">
         <v>2012</v>
       </c>
@@ -7144,7 +7136,7 @@
       <c r="K225" s="4"/>
       <c r="L225" s="4"/>
     </row>
-    <row r="226" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A226">
         <v>2012</v>
       </c>
@@ -7166,7 +7158,7 @@
       <c r="K226" s="4"/>
       <c r="L226" s="4"/>
     </row>
-    <row r="227" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A227">
         <v>2012</v>
       </c>
@@ -7188,7 +7180,7 @@
       <c r="K227" s="4"/>
       <c r="L227" s="4"/>
     </row>
-    <row r="228" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A228">
         <v>2012</v>
       </c>
@@ -7210,7 +7202,7 @@
       <c r="K228" s="4"/>
       <c r="L228" s="4"/>
     </row>
-    <row r="229" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A229">
         <v>2012</v>
       </c>
@@ -7234,7 +7226,7 @@
       <c r="K229" s="4"/>
       <c r="L229" s="4"/>
     </row>
-    <row r="230" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A230">
         <v>2012</v>
       </c>
@@ -7258,7 +7250,7 @@
       <c r="K230" s="4"/>
       <c r="L230" s="4"/>
     </row>
-    <row r="231" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A231">
         <v>2012</v>
       </c>
@@ -7282,7 +7274,7 @@
       <c r="K231" s="4"/>
       <c r="L231" s="4"/>
     </row>
-    <row r="232" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A232">
         <v>2012</v>
       </c>
@@ -7304,7 +7296,7 @@
       <c r="K232" s="4"/>
       <c r="L232" s="4"/>
     </row>
-    <row r="233" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A233">
         <v>2012</v>
       </c>
@@ -7326,7 +7318,7 @@
       <c r="K233" s="4"/>
       <c r="L233" s="4"/>
     </row>
-    <row r="234" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A234">
         <v>2012</v>
       </c>
@@ -7348,7 +7340,7 @@
       <c r="K234" s="4"/>
       <c r="L234" s="4"/>
     </row>
-    <row r="235" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A235">
         <v>2012</v>
       </c>
@@ -7370,7 +7362,7 @@
       <c r="K235" s="4"/>
       <c r="L235" s="4"/>
     </row>
-    <row r="236" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A236">
         <v>2012</v>
       </c>
@@ -7392,7 +7384,7 @@
       <c r="K236" s="4"/>
       <c r="L236" s="4"/>
     </row>
-    <row r="237" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A237">
         <v>2012</v>
       </c>
@@ -7414,7 +7406,7 @@
       <c r="K237" s="4"/>
       <c r="L237" s="4"/>
     </row>
-    <row r="238" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A238">
         <v>2012</v>
       </c>
@@ -7436,7 +7428,7 @@
       <c r="K238" s="4"/>
       <c r="L238" s="4"/>
     </row>
-    <row r="239" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A239">
         <v>2012</v>
       </c>
@@ -7458,7 +7450,7 @@
       <c r="K239" s="4"/>
       <c r="L239" s="4"/>
     </row>
-    <row r="240" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A240">
         <v>2012</v>
       </c>
@@ -7480,7 +7472,7 @@
       <c r="K240" s="4"/>
       <c r="L240" s="4"/>
     </row>
-    <row r="241" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A241">
         <v>2013</v>
       </c>
@@ -7504,7 +7496,7 @@
       <c r="K241" s="4"/>
       <c r="L241" s="4"/>
     </row>
-    <row r="242" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A242">
         <v>2013</v>
       </c>
@@ -7526,7 +7518,7 @@
       <c r="K242" s="4"/>
       <c r="L242" s="4"/>
     </row>
-    <row r="243" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A243">
         <v>2013</v>
       </c>
@@ -7550,7 +7542,7 @@
       <c r="K243" s="4"/>
       <c r="L243" s="4"/>
     </row>
-    <row r="244" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A244">
         <v>2013</v>
       </c>
@@ -7572,7 +7564,7 @@
       <c r="K244" s="4"/>
       <c r="L244" s="4"/>
     </row>
-    <row r="245" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A245">
         <v>2013</v>
       </c>
@@ -7596,7 +7588,7 @@
       <c r="K245" s="4"/>
       <c r="L245" s="4"/>
     </row>
-    <row r="246" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A246">
         <v>2013</v>
       </c>
@@ -7620,7 +7612,7 @@
       <c r="K246" s="4"/>
       <c r="L246" s="4"/>
     </row>
-    <row r="247" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A247">
         <v>2013</v>
       </c>
@@ -7644,7 +7636,7 @@
       <c r="K247" s="4"/>
       <c r="L247" s="4"/>
     </row>
-    <row r="248" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A248">
         <v>2013</v>
       </c>
@@ -7666,7 +7658,7 @@
       <c r="K248" s="4"/>
       <c r="L248" s="4"/>
     </row>
-    <row r="249" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A249">
         <v>2013</v>
       </c>
@@ -7688,7 +7680,7 @@
       <c r="K249" s="4"/>
       <c r="L249" s="4"/>
     </row>
-    <row r="250" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A250">
         <v>2013</v>
       </c>
@@ -7710,7 +7702,7 @@
       <c r="K250" s="4"/>
       <c r="L250" s="4"/>
     </row>
-    <row r="251" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A251">
         <v>2013</v>
       </c>
@@ -7732,7 +7724,7 @@
       <c r="K251" s="4"/>
       <c r="L251" s="4"/>
     </row>
-    <row r="252" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A252">
         <v>2013</v>
       </c>
@@ -7754,7 +7746,7 @@
       <c r="K252" s="4"/>
       <c r="L252" s="4"/>
     </row>
-    <row r="253" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A253">
         <v>2013</v>
       </c>
@@ -7778,7 +7770,7 @@
       <c r="K253" s="4"/>
       <c r="L253" s="4"/>
     </row>
-    <row r="254" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A254">
         <v>2013</v>
       </c>
@@ -7802,7 +7794,7 @@
       <c r="K254" s="4"/>
       <c r="L254" s="4"/>
     </row>
-    <row r="255" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A255">
         <v>2013</v>
       </c>
@@ -7824,7 +7816,7 @@
       <c r="K255" s="4"/>
       <c r="L255" s="4"/>
     </row>
-    <row r="256" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A256">
         <v>2013</v>
       </c>
@@ -7848,7 +7840,7 @@
       <c r="K256" s="4"/>
       <c r="L256" s="4"/>
     </row>
-    <row r="257" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A257">
         <v>2013</v>
       </c>
@@ -7870,7 +7862,7 @@
       <c r="K257" s="4"/>
       <c r="L257" s="4"/>
     </row>
-    <row r="258" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A258">
         <v>2013</v>
       </c>
@@ -7894,7 +7886,7 @@
       <c r="K258" s="4"/>
       <c r="L258" s="4"/>
     </row>
-    <row r="259" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A259">
         <v>2013</v>
       </c>
@@ -7918,7 +7910,7 @@
       <c r="K259" s="4"/>
       <c r="L259" s="4"/>
     </row>
-    <row r="260" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A260">
         <v>2013</v>
       </c>
@@ -7940,7 +7932,7 @@
       <c r="K260" s="4"/>
       <c r="L260" s="4"/>
     </row>
-    <row r="261" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A261">
         <v>2013</v>
       </c>
@@ -7964,7 +7956,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="262" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A262">
         <v>2013</v>
       </c>
@@ -7986,7 +7978,7 @@
       <c r="K262" s="4"/>
       <c r="L262" s="4"/>
     </row>
-    <row r="263" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A263">
         <v>2013</v>
       </c>
@@ -8008,7 +8000,7 @@
       <c r="K263" s="4"/>
       <c r="L263" s="4"/>
     </row>
-    <row r="264" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A264">
         <v>2013</v>
       </c>
@@ -8032,7 +8024,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="265" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A265">
         <v>2013</v>
       </c>
@@ -8054,7 +8046,7 @@
       <c r="K265" s="4"/>
       <c r="L265" s="4"/>
     </row>
-    <row r="266" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A266">
         <v>2013</v>
       </c>
@@ -8076,7 +8068,7 @@
       <c r="K266" s="4"/>
       <c r="L266" s="4"/>
     </row>
-    <row r="267" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A267">
         <v>2013</v>
       </c>
@@ -8100,7 +8092,7 @@
       </c>
       <c r="L267" s="4"/>
     </row>
-    <row r="268" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A268">
         <v>2013</v>
       </c>
@@ -8122,7 +8114,7 @@
       <c r="K268" s="4"/>
       <c r="L268" s="4"/>
     </row>
-    <row r="269" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A269">
         <v>2013</v>
       </c>
@@ -8144,7 +8136,7 @@
       <c r="K269" s="4"/>
       <c r="L269" s="4"/>
     </row>
-    <row r="270" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A270">
         <v>2013</v>
       </c>
@@ -8166,7 +8158,7 @@
       <c r="K270" s="4"/>
       <c r="L270" s="4"/>
     </row>
-    <row r="271" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A271">
         <v>2013</v>
       </c>
@@ -8188,7 +8180,7 @@
       <c r="K271" s="4"/>
       <c r="L271" s="4"/>
     </row>
-    <row r="272" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A272">
         <v>2013</v>
       </c>
@@ -8212,7 +8204,7 @@
       <c r="K272" s="4"/>
       <c r="L272" s="4"/>
     </row>
-    <row r="273" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A273">
         <v>2013</v>
       </c>
@@ -8234,7 +8226,7 @@
       <c r="K273" s="4"/>
       <c r="L273" s="4"/>
     </row>
-    <row r="274" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A274">
         <v>2013</v>
       </c>
@@ -8256,7 +8248,7 @@
       <c r="K274" s="4"/>
       <c r="L274" s="4"/>
     </row>
-    <row r="275" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A275">
         <v>2013</v>
       </c>
@@ -8278,7 +8270,7 @@
       <c r="K275" s="4"/>
       <c r="L275" s="4"/>
     </row>
-    <row r="276" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A276">
         <v>2013</v>
       </c>
@@ -8300,7 +8292,7 @@
       <c r="K276" s="4"/>
       <c r="L276" s="4"/>
     </row>
-    <row r="277" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A277">
         <v>2013</v>
       </c>
@@ -8322,7 +8314,7 @@
       <c r="K277" s="4"/>
       <c r="L277" s="4"/>
     </row>
-    <row r="278" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A278">
         <v>2013</v>
       </c>
@@ -8344,7 +8336,7 @@
       <c r="K278" s="4"/>
       <c r="L278" s="4"/>
     </row>
-    <row r="279" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A279">
         <v>2013</v>
       </c>
@@ -8368,7 +8360,7 @@
       <c r="K279" s="4"/>
       <c r="L279" s="4"/>
     </row>
-    <row r="280" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A280">
         <v>2013</v>
       </c>
@@ -8392,7 +8384,7 @@
       <c r="K280" s="4"/>
       <c r="L280" s="4"/>
     </row>
-    <row r="281" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A281">
         <v>2013</v>
       </c>
@@ -8416,7 +8408,7 @@
       <c r="K281" s="4"/>
       <c r="L281" s="4"/>
     </row>
-    <row r="282" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A282">
         <v>2013</v>
       </c>
@@ -8438,7 +8430,7 @@
       <c r="K282" s="4"/>
       <c r="L282" s="4"/>
     </row>
-    <row r="283" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A283">
         <v>2013</v>
       </c>
@@ -8460,7 +8452,7 @@
       <c r="K283" s="4"/>
       <c r="L283" s="4"/>
     </row>
-    <row r="284" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A284">
         <v>2013</v>
       </c>
@@ -8482,7 +8474,7 @@
       <c r="K284" s="4"/>
       <c r="L284" s="4"/>
     </row>
-    <row r="285" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A285">
         <v>2013</v>
       </c>
@@ -8504,7 +8496,7 @@
       <c r="K285" s="4"/>
       <c r="L285" s="4"/>
     </row>
-    <row r="286" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A286">
         <v>2013</v>
       </c>
@@ -8526,7 +8518,7 @@
       <c r="K286" s="4"/>
       <c r="L286" s="4"/>
     </row>
-    <row r="287" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A287">
         <v>2013</v>
       </c>
@@ -8548,7 +8540,7 @@
       <c r="K287" s="4"/>
       <c r="L287" s="4"/>
     </row>
-    <row r="288" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A288">
         <v>2013</v>
       </c>
@@ -8570,7 +8562,7 @@
       <c r="K288" s="4"/>
       <c r="L288" s="4"/>
     </row>
-    <row r="289" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A289">
         <v>2013</v>
       </c>
@@ -8592,7 +8584,7 @@
       <c r="K289" s="4"/>
       <c r="L289" s="4"/>
     </row>
-    <row r="290" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A290">
         <v>2013</v>
       </c>
@@ -8614,7 +8606,7 @@
       <c r="K290" s="4"/>
       <c r="L290" s="4"/>
     </row>
-    <row r="291" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A291">
         <v>2014</v>
       </c>
@@ -8638,7 +8630,7 @@
       <c r="K291" s="4"/>
       <c r="L291" s="4"/>
     </row>
-    <row r="292" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A292">
         <v>2014</v>
       </c>
@@ -8662,7 +8654,7 @@
       <c r="K292" s="4"/>
       <c r="L292" s="4"/>
     </row>
-    <row r="293" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A293">
         <v>2014</v>
       </c>
@@ -8686,7 +8678,7 @@
       <c r="K293" s="4"/>
       <c r="L293" s="4"/>
     </row>
-    <row r="294" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A294">
         <v>2014</v>
       </c>
@@ -8708,7 +8700,7 @@
       <c r="K294" s="4"/>
       <c r="L294" s="4"/>
     </row>
-    <row r="295" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A295">
         <v>2014</v>
       </c>
@@ -8732,7 +8724,7 @@
       <c r="K295" s="4"/>
       <c r="L295" s="4"/>
     </row>
-    <row r="296" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A296">
         <v>2014</v>
       </c>
@@ -8754,7 +8746,7 @@
       <c r="K296" s="4"/>
       <c r="L296" s="4"/>
     </row>
-    <row r="297" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A297">
         <v>2014</v>
       </c>
@@ -8778,7 +8770,7 @@
       <c r="K297" s="4"/>
       <c r="L297" s="4"/>
     </row>
-    <row r="298" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A298">
         <v>2014</v>
       </c>
@@ -8802,7 +8794,7 @@
       <c r="K298" s="4"/>
       <c r="L298" s="4"/>
     </row>
-    <row r="299" spans="1:12" ht="36" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:12" ht="36" x14ac:dyDescent="0.3">
       <c r="A299">
         <v>2014</v>
       </c>
@@ -8826,7 +8818,7 @@
       <c r="K299" s="4"/>
       <c r="L299" s="4"/>
     </row>
-    <row r="300" spans="1:12" ht="36" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A300">
         <v>2014</v>
       </c>
@@ -8850,7 +8842,7 @@
       <c r="K300" s="4"/>
       <c r="L300" s="4"/>
     </row>
-    <row r="301" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A301">
         <v>2014</v>
       </c>
@@ -8874,7 +8866,7 @@
       <c r="K301" s="4"/>
       <c r="L301" s="4"/>
     </row>
-    <row r="302" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A302">
         <v>2014</v>
       </c>
@@ -8896,7 +8888,7 @@
       <c r="K302" s="4"/>
       <c r="L302" s="4"/>
     </row>
-    <row r="303" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A303">
         <v>2014</v>
       </c>
@@ -8920,7 +8912,7 @@
       <c r="K303" s="4"/>
       <c r="L303" s="4"/>
     </row>
-    <row r="304" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A304">
         <v>2014</v>
       </c>
@@ -8942,7 +8934,7 @@
       <c r="K304" s="4"/>
       <c r="L304" s="4"/>
     </row>
-    <row r="305" spans="1:12" ht="36" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:12" ht="36" x14ac:dyDescent="0.3">
       <c r="A305">
         <v>2014</v>
       </c>
@@ -8966,7 +8958,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="306" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A306">
         <v>2014</v>
       </c>
@@ -8988,7 +8980,7 @@
       <c r="K306" s="4"/>
       <c r="L306" s="4"/>
     </row>
-    <row r="307" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A307">
         <v>2014</v>
       </c>
@@ -9010,7 +9002,7 @@
       <c r="K307" s="4"/>
       <c r="L307" s="4"/>
     </row>
-    <row r="308" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A308">
         <v>2014</v>
       </c>
@@ -9032,7 +9024,7 @@
       <c r="K308" s="4"/>
       <c r="L308" s="4"/>
     </row>
-    <row r="309" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A309">
         <v>2014</v>
       </c>
@@ -9054,7 +9046,7 @@
       <c r="K309" s="4"/>
       <c r="L309" s="4"/>
     </row>
-    <row r="310" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A310">
         <v>2014</v>
       </c>
@@ -9078,7 +9070,7 @@
       </c>
       <c r="L310" s="4"/>
     </row>
-    <row r="311" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A311">
         <v>2014</v>
       </c>
@@ -9102,7 +9094,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="312" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A312">
         <v>2014</v>
       </c>
@@ -9126,7 +9118,7 @@
       <c r="K312" s="4"/>
       <c r="L312" s="4"/>
     </row>
-    <row r="313" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A313">
         <v>2014</v>
       </c>
@@ -9150,7 +9142,7 @@
       <c r="K313" s="4"/>
       <c r="L313" s="4"/>
     </row>
-    <row r="314" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A314">
         <v>2014</v>
       </c>
@@ -9172,7 +9164,7 @@
       <c r="K314" s="4"/>
       <c r="L314" s="4"/>
     </row>
-    <row r="315" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A315">
         <v>2014</v>
       </c>
@@ -9194,7 +9186,7 @@
       <c r="K315" s="4"/>
       <c r="L315" s="4"/>
     </row>
-    <row r="316" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A316">
         <v>2014</v>
       </c>
@@ -9216,7 +9208,7 @@
       <c r="K316" s="4"/>
       <c r="L316" s="4"/>
     </row>
-    <row r="317" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A317">
         <v>2014</v>
       </c>
@@ -9238,7 +9230,7 @@
       <c r="K317" s="4"/>
       <c r="L317" s="4"/>
     </row>
-    <row r="318" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:12" ht="36" x14ac:dyDescent="0.3">
       <c r="A318">
         <v>2014</v>
       </c>
@@ -9260,7 +9252,7 @@
       <c r="K318" s="4"/>
       <c r="L318" s="4"/>
     </row>
-    <row r="319" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A319">
         <v>2014</v>
       </c>
@@ -9284,7 +9276,7 @@
       <c r="K319" s="4"/>
       <c r="L319" s="4"/>
     </row>
-    <row r="320" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A320">
         <v>2014</v>
       </c>
@@ -9306,7 +9298,7 @@
       <c r="K320" s="4"/>
       <c r="L320" s="4"/>
     </row>
-    <row r="321" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A321">
         <v>2014</v>
       </c>
@@ -9328,7 +9320,7 @@
       <c r="K321" s="4"/>
       <c r="L321" s="4"/>
     </row>
-    <row r="322" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A322">
         <v>2015</v>
       </c>
@@ -9352,7 +9344,7 @@
       <c r="K322" s="4"/>
       <c r="L322" s="4"/>
     </row>
-    <row r="323" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A323">
         <v>2015</v>
       </c>
@@ -9374,7 +9366,7 @@
       <c r="K323" s="4"/>
       <c r="L323" s="4"/>
     </row>
-    <row r="324" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A324">
         <v>2015</v>
       </c>
@@ -9398,7 +9390,7 @@
       <c r="K324" s="4"/>
       <c r="L324" s="4"/>
     </row>
-    <row r="325" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A325">
         <v>2015</v>
       </c>
@@ -9422,7 +9414,7 @@
       <c r="K325" s="4"/>
       <c r="L325" s="4"/>
     </row>
-    <row r="326" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A326">
         <v>2015</v>
       </c>
@@ -9446,7 +9438,7 @@
       <c r="K326" s="4"/>
       <c r="L326" s="4"/>
     </row>
-    <row r="327" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A327">
         <v>2015</v>
       </c>
@@ -9468,7 +9460,7 @@
       <c r="K327" s="4"/>
       <c r="L327" s="4"/>
     </row>
-    <row r="328" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A328">
         <v>2015</v>
       </c>
@@ -9492,7 +9484,7 @@
       <c r="K328" s="4"/>
       <c r="L328" s="4"/>
     </row>
-    <row r="329" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A329">
         <v>2015</v>
       </c>
@@ -9514,7 +9506,7 @@
       <c r="K329" s="4"/>
       <c r="L329" s="4"/>
     </row>
-    <row r="330" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A330">
         <v>2015</v>
       </c>
@@ -9538,7 +9530,7 @@
       <c r="K330" s="4"/>
       <c r="L330" s="4"/>
     </row>
-    <row r="331" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A331">
         <v>2015</v>
       </c>
@@ -9560,7 +9552,7 @@
       <c r="K331" s="4"/>
       <c r="L331" s="4"/>
     </row>
-    <row r="332" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A332">
         <v>2015</v>
       </c>
@@ -9584,7 +9576,7 @@
       <c r="K332" s="4"/>
       <c r="L332" s="4"/>
     </row>
-    <row r="333" spans="1:12" ht="36" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:12" ht="36" x14ac:dyDescent="0.3">
       <c r="A333">
         <v>2015</v>
       </c>
@@ -9608,7 +9600,7 @@
       <c r="K333" s="4"/>
       <c r="L333" s="4"/>
     </row>
-    <row r="334" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A334">
         <v>2015</v>
       </c>
@@ -9632,7 +9624,7 @@
       <c r="K334" s="4"/>
       <c r="L334" s="4"/>
     </row>
-    <row r="335" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A335">
         <v>2015</v>
       </c>
@@ -9654,7 +9646,7 @@
       <c r="K335" s="4"/>
       <c r="L335" s="4"/>
     </row>
-    <row r="336" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A336">
         <v>2015</v>
       </c>
@@ -9678,7 +9670,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="337" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A337">
         <v>2015</v>
       </c>
@@ -9702,7 +9694,7 @@
       </c>
       <c r="L337" s="4"/>
     </row>
-    <row r="338" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A338">
         <v>2015</v>
       </c>
@@ -9726,7 +9718,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="339" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A339">
         <v>2015</v>
       </c>
@@ -9748,7 +9740,7 @@
       <c r="K339" s="4"/>
       <c r="L339" s="4"/>
     </row>
-    <row r="340" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A340">
         <v>2015</v>
       </c>
@@ -9770,7 +9762,7 @@
       <c r="K340" s="4"/>
       <c r="L340" s="4"/>
     </row>
-    <row r="341" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A341">
         <v>2015</v>
       </c>
@@ -9794,7 +9786,7 @@
       <c r="K341" s="4"/>
       <c r="L341" s="4"/>
     </row>
-    <row r="342" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A342">
         <v>2015</v>
       </c>
@@ -9816,7 +9808,7 @@
       <c r="K342" s="4"/>
       <c r="L342" s="4"/>
     </row>
-    <row r="343" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A343">
         <v>2015</v>
       </c>
@@ -9838,7 +9830,7 @@
       <c r="K343" s="4"/>
       <c r="L343" s="4"/>
     </row>
-    <row r="344" spans="1:12" ht="36" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:12" ht="36" x14ac:dyDescent="0.3">
       <c r="A344">
         <v>2015</v>
       </c>
@@ -9862,7 +9854,7 @@
       <c r="K344" s="4"/>
       <c r="L344" s="4"/>
     </row>
-    <row r="345" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A345">
         <v>2015</v>
       </c>
@@ -9886,7 +9878,7 @@
       <c r="K345" s="4"/>
       <c r="L345" s="4"/>
     </row>
-    <row r="346" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A346">
         <v>2015</v>
       </c>
@@ -9908,7 +9900,7 @@
       <c r="K346" s="4"/>
       <c r="L346" s="4"/>
     </row>
-    <row r="347" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A347">
         <v>2015</v>
       </c>
@@ -9932,7 +9924,7 @@
       <c r="K347" s="4"/>
       <c r="L347" s="4"/>
     </row>
-    <row r="348" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A348">
         <v>2015</v>
       </c>
@@ -9954,7 +9946,7 @@
       <c r="K348" s="4"/>
       <c r="L348" s="4"/>
     </row>
-    <row r="349" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A349">
         <v>2015</v>
       </c>
@@ -9976,7 +9968,7 @@
       <c r="K349" s="4"/>
       <c r="L349" s="4"/>
     </row>
-    <row r="350" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A350">
         <v>2016</v>
       </c>
@@ -10000,7 +9992,7 @@
       <c r="K350" s="4"/>
       <c r="L350" s="4"/>
     </row>
-    <row r="351" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A351">
         <v>2016</v>
       </c>
@@ -10022,7 +10014,7 @@
       <c r="K351" s="4"/>
       <c r="L351" s="4"/>
     </row>
-    <row r="352" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A352">
         <v>2016</v>
       </c>
@@ -10046,7 +10038,7 @@
       <c r="K352" s="4"/>
       <c r="L352" s="4"/>
     </row>
-    <row r="353" spans="1:12" ht="36" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:12" ht="36" x14ac:dyDescent="0.3">
       <c r="A353">
         <v>2016</v>
       </c>
@@ -10070,7 +10062,7 @@
       <c r="K353" s="4"/>
       <c r="L353" s="4"/>
     </row>
-    <row r="354" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A354">
         <v>2016</v>
       </c>
@@ -10094,7 +10086,7 @@
       <c r="K354" s="4"/>
       <c r="L354" s="4"/>
     </row>
-    <row r="355" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A355">
         <v>2016</v>
       </c>
@@ -10116,7 +10108,7 @@
       <c r="K355" s="4"/>
       <c r="L355" s="4"/>
     </row>
-    <row r="356" spans="1:12" ht="36" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:12" ht="36" x14ac:dyDescent="0.3">
       <c r="A356">
         <v>2016</v>
       </c>
@@ -10138,7 +10130,7 @@
       <c r="K356" s="4"/>
       <c r="L356" s="4"/>
     </row>
-    <row r="357" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A357">
         <v>2016</v>
       </c>
@@ -10162,7 +10154,7 @@
       <c r="K357" s="4"/>
       <c r="L357" s="4"/>
     </row>
-    <row r="358" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A358">
         <v>2016</v>
       </c>
@@ -10184,7 +10176,7 @@
       <c r="K358" s="4"/>
       <c r="L358" s="4"/>
     </row>
-    <row r="359" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A359">
         <v>2016</v>
       </c>
@@ -10208,7 +10200,7 @@
       <c r="K359" s="4"/>
       <c r="L359" s="4"/>
     </row>
-    <row r="360" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A360">
         <v>2016</v>
       </c>
@@ -10230,7 +10222,7 @@
       <c r="K360" s="4"/>
       <c r="L360" s="4"/>
     </row>
-    <row r="361" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A361">
         <v>2016</v>
       </c>
@@ -10254,7 +10246,7 @@
       <c r="K361" s="4"/>
       <c r="L361" s="4"/>
     </row>
-    <row r="362" spans="1:12" ht="36" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:12" ht="36" x14ac:dyDescent="0.3">
       <c r="A362">
         <v>2016</v>
       </c>
@@ -10278,7 +10270,7 @@
       <c r="K362" s="4"/>
       <c r="L362" s="4"/>
     </row>
-    <row r="363" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A363">
         <v>2016</v>
       </c>
@@ -10302,7 +10294,7 @@
       <c r="K363" s="4"/>
       <c r="L363" s="4"/>
     </row>
-    <row r="364" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A364">
         <v>2016</v>
       </c>
@@ -10324,7 +10316,7 @@
       <c r="K364" s="4"/>
       <c r="L364" s="4"/>
     </row>
-    <row r="365" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A365">
         <v>2016</v>
       </c>
@@ -10348,7 +10340,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="366" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A366">
         <v>2016</v>
       </c>
@@ -10372,7 +10364,7 @@
       </c>
       <c r="L366" s="4"/>
     </row>
-    <row r="367" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A367">
         <v>2016</v>
       </c>
@@ -10396,7 +10388,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="368" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A368">
         <v>2016</v>
       </c>
@@ -10418,7 +10410,7 @@
       <c r="K368" s="4"/>
       <c r="L368" s="4"/>
     </row>
-    <row r="369" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A369">
         <v>2016</v>
       </c>
@@ -10440,7 +10432,7 @@
       <c r="K369" s="4"/>
       <c r="L369" s="4"/>
     </row>
-    <row r="370" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A370">
         <v>2016</v>
       </c>
@@ -10464,7 +10456,7 @@
       <c r="K370" s="4"/>
       <c r="L370" s="4"/>
     </row>
-    <row r="371" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A371">
         <v>2016</v>
       </c>
@@ -10486,7 +10478,7 @@
       <c r="K371" s="4"/>
       <c r="L371" s="4"/>
     </row>
-    <row r="372" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A372">
         <v>2016</v>
       </c>
@@ -10508,7 +10500,7 @@
       <c r="K372" s="4"/>
       <c r="L372" s="4"/>
     </row>
-    <row r="373" spans="1:12" ht="36" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:12" ht="36" x14ac:dyDescent="0.3">
       <c r="A373">
         <v>2016</v>
       </c>
@@ -10532,7 +10524,7 @@
       <c r="K373" s="4"/>
       <c r="L373" s="4"/>
     </row>
-    <row r="374" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A374">
         <v>2016</v>
       </c>
@@ -10554,7 +10546,7 @@
       <c r="K374" s="4"/>
       <c r="L374" s="4"/>
     </row>
-    <row r="375" spans="1:12" ht="36" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:12" ht="36" x14ac:dyDescent="0.3">
       <c r="A375">
         <v>2016</v>
       </c>
@@ -10576,7 +10568,7 @@
       <c r="K375" s="4"/>
       <c r="L375" s="4"/>
     </row>
-    <row r="376" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A376">
         <v>2016</v>
       </c>
@@ -10600,7 +10592,7 @@
       <c r="K376" s="4"/>
       <c r="L376" s="4"/>
     </row>
-    <row r="377" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A377">
         <v>2016</v>
       </c>
@@ -10622,7 +10614,7 @@
       <c r="K377" s="4"/>
       <c r="L377" s="4"/>
     </row>
-    <row r="378" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A378">
         <v>2016</v>
       </c>
@@ -10644,7 +10636,7 @@
       <c r="K378" s="4"/>
       <c r="L378" s="4"/>
     </row>
-    <row r="379" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A379">
         <v>2017</v>
       </c>
@@ -10668,7 +10660,7 @@
       <c r="K379" s="4"/>
       <c r="L379" s="4"/>
     </row>
-    <row r="380" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A380">
         <v>2017</v>
       </c>
@@ -10690,7 +10682,7 @@
       <c r="K380" s="4"/>
       <c r="L380" s="4"/>
     </row>
-    <row r="381" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A381">
         <v>2017</v>
       </c>
@@ -10714,7 +10706,7 @@
       <c r="K381" s="4"/>
       <c r="L381" s="4"/>
     </row>
-    <row r="382" spans="1:12" ht="36" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:12" ht="36" x14ac:dyDescent="0.3">
       <c r="A382">
         <v>2017</v>
       </c>
@@ -10738,7 +10730,7 @@
       <c r="K382" s="4"/>
       <c r="L382" s="4"/>
     </row>
-    <row r="383" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A383">
         <v>2017</v>
       </c>
@@ -10762,7 +10754,7 @@
       <c r="K383" s="4"/>
       <c r="L383" s="4"/>
     </row>
-    <row r="384" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A384">
         <v>2017</v>
       </c>
@@ -10784,7 +10776,7 @@
       <c r="K384" s="4"/>
       <c r="L384" s="4"/>
     </row>
-    <row r="385" spans="1:12" ht="36" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:12" ht="36" x14ac:dyDescent="0.3">
       <c r="A385">
         <v>2017</v>
       </c>
@@ -10806,7 +10798,7 @@
       <c r="K385" s="4"/>
       <c r="L385" s="4"/>
     </row>
-    <row r="386" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A386">
         <v>2017</v>
       </c>
@@ -10830,7 +10822,7 @@
       <c r="K386" s="4"/>
       <c r="L386" s="4"/>
     </row>
-    <row r="387" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A387">
         <v>2017</v>
       </c>
@@ -10852,7 +10844,7 @@
       <c r="K387" s="4"/>
       <c r="L387" s="4"/>
     </row>
-    <row r="388" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A388">
         <v>2017</v>
       </c>
@@ -10876,7 +10868,7 @@
       <c r="K388" s="4"/>
       <c r="L388" s="4"/>
     </row>
-    <row r="389" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A389">
         <v>2017</v>
       </c>
@@ -10898,7 +10890,7 @@
       <c r="K389" s="4"/>
       <c r="L389" s="4"/>
     </row>
-    <row r="390" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A390">
         <v>2017</v>
       </c>
@@ -10922,7 +10914,7 @@
       <c r="K390" s="4"/>
       <c r="L390" s="4"/>
     </row>
-    <row r="391" spans="1:12" ht="36" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:12" ht="36" x14ac:dyDescent="0.3">
       <c r="A391">
         <v>2017</v>
       </c>
@@ -10946,7 +10938,7 @@
       <c r="K391" s="4"/>
       <c r="L391" s="4"/>
     </row>
-    <row r="392" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A392">
         <v>2017</v>
       </c>
@@ -10970,7 +10962,7 @@
       <c r="K392" s="4"/>
       <c r="L392" s="4"/>
     </row>
-    <row r="393" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A393">
         <v>2017</v>
       </c>
@@ -10992,7 +10984,7 @@
       <c r="K393" s="4"/>
       <c r="L393" s="4"/>
     </row>
-    <row r="394" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A394">
         <v>2017</v>
       </c>
@@ -11014,7 +11006,7 @@
       <c r="K394" s="4"/>
       <c r="L394" s="4"/>
     </row>
-    <row r="395" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A395">
         <v>2017</v>
       </c>
@@ -11038,7 +11030,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="396" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A396">
         <v>2017</v>
       </c>
@@ -11062,7 +11054,7 @@
       </c>
       <c r="L396" s="4"/>
     </row>
-    <row r="397" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A397">
         <v>2017</v>
       </c>
@@ -11086,7 +11078,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="398" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A398">
         <v>2017</v>
       </c>
@@ -11108,7 +11100,7 @@
       <c r="K398" s="4"/>
       <c r="L398" s="4"/>
     </row>
-    <row r="399" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A399">
         <v>2017</v>
       </c>
@@ -11130,7 +11122,7 @@
       <c r="K399" s="4"/>
       <c r="L399" s="4"/>
     </row>
-    <row r="400" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A400">
         <v>2017</v>
       </c>
@@ -11154,7 +11146,7 @@
       <c r="K400" s="4"/>
       <c r="L400" s="4"/>
     </row>
-    <row r="401" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A401">
         <v>2017</v>
       </c>
@@ -11176,7 +11168,7 @@
       <c r="K401" s="4"/>
       <c r="L401" s="4"/>
     </row>
-    <row r="402" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A402">
         <v>2017</v>
       </c>
@@ -11198,7 +11190,7 @@
       <c r="K402" s="4"/>
       <c r="L402" s="4"/>
     </row>
-    <row r="403" spans="1:12" ht="36" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:12" ht="36" x14ac:dyDescent="0.3">
       <c r="A403">
         <v>2017</v>
       </c>
@@ -11222,7 +11214,7 @@
       <c r="K403" s="4"/>
       <c r="L403" s="4"/>
     </row>
-    <row r="404" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A404">
         <v>2017</v>
       </c>
@@ -11244,7 +11236,7 @@
       <c r="K404" s="4"/>
       <c r="L404" s="4"/>
     </row>
-    <row r="405" spans="1:12" ht="36" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:12" ht="36" x14ac:dyDescent="0.3">
       <c r="A405">
         <v>2017</v>
       </c>
@@ -11266,7 +11258,7 @@
       <c r="K405" s="4"/>
       <c r="L405" s="4"/>
     </row>
-    <row r="406" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A406">
         <v>2017</v>
       </c>
@@ -11290,7 +11282,7 @@
       <c r="K406" s="4"/>
       <c r="L406" s="4"/>
     </row>
-    <row r="407" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A407">
         <v>2017</v>
       </c>
@@ -11312,7 +11304,7 @@
       <c r="K407" s="4"/>
       <c r="L407" s="4"/>
     </row>
-    <row r="408" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A408">
         <v>2017</v>
       </c>
@@ -11334,7 +11326,7 @@
       <c r="K408" s="4"/>
       <c r="L408" s="4"/>
     </row>
-    <row r="409" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A409">
         <v>2018</v>
       </c>
@@ -11358,7 +11350,7 @@
       <c r="K409" s="4"/>
       <c r="L409" s="4"/>
     </row>
-    <row r="410" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A410">
         <v>2018</v>
       </c>
@@ -11380,7 +11372,7 @@
       <c r="K410" s="4"/>
       <c r="L410" s="4"/>
     </row>
-    <row r="411" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A411">
         <v>2018</v>
       </c>
@@ -11404,7 +11396,7 @@
       <c r="K411" s="4"/>
       <c r="L411" s="4"/>
     </row>
-    <row r="412" spans="1:12" ht="36" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:12" ht="36" x14ac:dyDescent="0.3">
       <c r="A412">
         <v>2018</v>
       </c>
@@ -11428,7 +11420,7 @@
       <c r="K412" s="4"/>
       <c r="L412" s="4"/>
     </row>
-    <row r="413" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A413">
         <v>2018</v>
       </c>
@@ -11452,7 +11444,7 @@
       <c r="K413" s="4"/>
       <c r="L413" s="4"/>
     </row>
-    <row r="414" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A414">
         <v>2018</v>
       </c>
@@ -11474,7 +11466,7 @@
       <c r="K414" s="4"/>
       <c r="L414" s="4"/>
     </row>
-    <row r="415" spans="1:12" ht="36" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:12" ht="36" x14ac:dyDescent="0.3">
       <c r="A415">
         <v>2018</v>
       </c>
@@ -11496,7 +11488,7 @@
       <c r="K415" s="4"/>
       <c r="L415" s="4"/>
     </row>
-    <row r="416" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A416">
         <v>2018</v>
       </c>
@@ -11520,7 +11512,7 @@
       <c r="K416" s="4"/>
       <c r="L416" s="4"/>
     </row>
-    <row r="417" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A417">
         <v>2018</v>
       </c>
@@ -11542,7 +11534,7 @@
       <c r="K417" s="4"/>
       <c r="L417" s="4"/>
     </row>
-    <row r="418" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A418">
         <v>2018</v>
       </c>
@@ -11566,7 +11558,7 @@
       <c r="K418" s="4"/>
       <c r="L418" s="4"/>
     </row>
-    <row r="419" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A419">
         <v>2018</v>
       </c>
@@ -11588,7 +11580,7 @@
       <c r="K419" s="4"/>
       <c r="L419" s="4"/>
     </row>
-    <row r="420" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A420">
         <v>2018</v>
       </c>
@@ -11612,7 +11604,7 @@
       <c r="K420" s="4"/>
       <c r="L420" s="4"/>
     </row>
-    <row r="421" spans="1:12" ht="36" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:12" ht="36" x14ac:dyDescent="0.3">
       <c r="A421">
         <v>2018</v>
       </c>
@@ -11636,7 +11628,7 @@
       <c r="K421" s="4"/>
       <c r="L421" s="4"/>
     </row>
-    <row r="422" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A422">
         <v>2018</v>
       </c>
@@ -11660,7 +11652,7 @@
       <c r="K422" s="4"/>
       <c r="L422" s="4"/>
     </row>
-    <row r="423" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A423">
         <v>2018</v>
       </c>
@@ -11682,7 +11674,7 @@
       <c r="K423" s="4"/>
       <c r="L423" s="4"/>
     </row>
-    <row r="424" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A424">
         <v>2018</v>
       </c>
@@ -11704,7 +11696,7 @@
       <c r="K424" s="4"/>
       <c r="L424" s="4"/>
     </row>
-    <row r="425" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A425">
         <v>2018</v>
       </c>
@@ -11728,7 +11720,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="426" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A426">
         <v>2018</v>
       </c>
@@ -11752,7 +11744,7 @@
       </c>
       <c r="L426" s="4"/>
     </row>
-    <row r="427" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A427">
         <v>2018</v>
       </c>
@@ -11776,7 +11768,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="428" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A428">
         <v>2018</v>
       </c>
@@ -11798,7 +11790,7 @@
       <c r="K428" s="4"/>
       <c r="L428" s="4"/>
     </row>
-    <row r="429" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A429">
         <v>2018</v>
       </c>
@@ -11820,7 +11812,7 @@
       <c r="K429" s="4"/>
       <c r="L429" s="4"/>
     </row>
-    <row r="430" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A430">
         <v>2018</v>
       </c>
@@ -11844,7 +11836,7 @@
       <c r="K430" s="4"/>
       <c r="L430" s="4"/>
     </row>
-    <row r="431" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A431">
         <v>2018</v>
       </c>
@@ -11866,7 +11858,7 @@
       <c r="K431" s="4"/>
       <c r="L431" s="4"/>
     </row>
-    <row r="432" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A432">
         <v>2018</v>
       </c>
@@ -11888,7 +11880,7 @@
       <c r="K432" s="4"/>
       <c r="L432" s="4"/>
     </row>
-    <row r="433" spans="1:12" ht="36" x14ac:dyDescent="0.25">
+    <row r="433" spans="1:12" ht="36" x14ac:dyDescent="0.3">
       <c r="A433">
         <v>2018</v>
       </c>
@@ -11912,7 +11904,7 @@
       <c r="K433" s="4"/>
       <c r="L433" s="4"/>
     </row>
-    <row r="434" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="434" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A434">
         <v>2018</v>
       </c>
@@ -11934,7 +11926,7 @@
       <c r="K434" s="4"/>
       <c r="L434" s="4"/>
     </row>
-    <row r="435" spans="1:12" ht="36" x14ac:dyDescent="0.25">
+    <row r="435" spans="1:12" ht="36" x14ac:dyDescent="0.3">
       <c r="A435">
         <v>2018</v>
       </c>
@@ -11956,7 +11948,7 @@
       <c r="K435" s="4"/>
       <c r="L435" s="4"/>
     </row>
-    <row r="436" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A436">
         <v>2018</v>
       </c>
@@ -11980,7 +11972,7 @@
       <c r="K436" s="4"/>
       <c r="L436" s="4"/>
     </row>
-    <row r="437" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A437">
         <v>2018</v>
       </c>
@@ -12002,7 +11994,7 @@
       <c r="K437" s="4"/>
       <c r="L437" s="4"/>
     </row>
-    <row r="438" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A438">
         <v>2018</v>
       </c>
@@ -12024,7 +12016,7 @@
       <c r="K438" s="4"/>
       <c r="L438" s="4"/>
     </row>
-    <row r="439" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="439" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A439">
         <v>2019</v>
       </c>
@@ -12048,7 +12040,7 @@
       <c r="K439" s="4"/>
       <c r="L439" s="4"/>
     </row>
-    <row r="440" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="440" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A440">
         <v>2019</v>
       </c>
@@ -12070,7 +12062,7 @@
       <c r="K440" s="4"/>
       <c r="L440" s="4"/>
     </row>
-    <row r="441" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A441">
         <v>2019</v>
       </c>
@@ -12094,7 +12086,7 @@
       <c r="K441" s="4"/>
       <c r="L441" s="4"/>
     </row>
-    <row r="442" spans="1:12" ht="36" x14ac:dyDescent="0.25">
+    <row r="442" spans="1:12" ht="36" x14ac:dyDescent="0.3">
       <c r="A442">
         <v>2019</v>
       </c>
@@ -12118,7 +12110,7 @@
       <c r="K442" s="4"/>
       <c r="L442" s="4"/>
     </row>
-    <row r="443" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="443" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A443">
         <v>2019</v>
       </c>
@@ -12142,7 +12134,7 @@
       <c r="K443" s="4"/>
       <c r="L443" s="4"/>
     </row>
-    <row r="444" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="444" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A444">
         <v>2019</v>
       </c>
@@ -12164,7 +12156,7 @@
       <c r="K444" s="4"/>
       <c r="L444" s="4"/>
     </row>
-    <row r="445" spans="1:12" ht="36" x14ac:dyDescent="0.25">
+    <row r="445" spans="1:12" ht="36" x14ac:dyDescent="0.3">
       <c r="A445">
         <v>2019</v>
       </c>
@@ -12186,7 +12178,7 @@
       <c r="K445" s="4"/>
       <c r="L445" s="4"/>
     </row>
-    <row r="446" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="446" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A446">
         <v>2019</v>
       </c>
@@ -12210,7 +12202,7 @@
       <c r="K446" s="4"/>
       <c r="L446" s="4"/>
     </row>
-    <row r="447" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="447" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A447">
         <v>2019</v>
       </c>
@@ -12232,7 +12224,7 @@
       <c r="K447" s="4"/>
       <c r="L447" s="4"/>
     </row>
-    <row r="448" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="448" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A448">
         <v>2019</v>
       </c>
@@ -12256,7 +12248,7 @@
       <c r="K448" s="4"/>
       <c r="L448" s="4"/>
     </row>
-    <row r="449" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="449" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A449">
         <v>2019</v>
       </c>
@@ -12278,7 +12270,7 @@
       <c r="K449" s="4"/>
       <c r="L449" s="4"/>
     </row>
-    <row r="450" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="450" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A450">
         <v>2019</v>
       </c>
@@ -12302,7 +12294,7 @@
       <c r="K450" s="4"/>
       <c r="L450" s="4"/>
     </row>
-    <row r="451" spans="1:12" ht="36" x14ac:dyDescent="0.25">
+    <row r="451" spans="1:12" ht="36" x14ac:dyDescent="0.3">
       <c r="A451">
         <v>2019</v>
       </c>
@@ -12326,7 +12318,7 @@
       <c r="K451" s="4"/>
       <c r="L451" s="4"/>
     </row>
-    <row r="452" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="452" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A452">
         <v>2019</v>
       </c>
@@ -12350,7 +12342,7 @@
       <c r="K452" s="4"/>
       <c r="L452" s="4"/>
     </row>
-    <row r="453" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="453" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A453">
         <v>2019</v>
       </c>
@@ -12372,7 +12364,7 @@
       <c r="K453" s="4"/>
       <c r="L453" s="4"/>
     </row>
-    <row r="454" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="454" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A454">
         <v>2019</v>
       </c>
@@ -12394,7 +12386,7 @@
       <c r="K454" s="4"/>
       <c r="L454" s="4"/>
     </row>
-    <row r="455" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="455" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A455">
         <v>2019</v>
       </c>
@@ -12418,7 +12410,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="456" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="456" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A456">
         <v>2019</v>
       </c>
@@ -12442,7 +12434,7 @@
       </c>
       <c r="L456" s="4"/>
     </row>
-    <row r="457" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="457" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A457">
         <v>2019</v>
       </c>
@@ -12466,7 +12458,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="458" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="458" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A458">
         <v>2019</v>
       </c>
@@ -12488,7 +12480,7 @@
       <c r="K458" s="4"/>
       <c r="L458" s="4"/>
     </row>
-    <row r="459" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="459" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A459">
         <v>2019</v>
       </c>
@@ -12510,7 +12502,7 @@
       <c r="K459" s="4"/>
       <c r="L459" s="4"/>
     </row>
-    <row r="460" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="460" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A460">
         <v>2019</v>
       </c>
@@ -12534,7 +12526,7 @@
       <c r="K460" s="4"/>
       <c r="L460" s="4"/>
     </row>
-    <row r="461" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="461" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A461">
         <v>2019</v>
       </c>
@@ -12556,7 +12548,7 @@
       <c r="K461" s="4"/>
       <c r="L461" s="4"/>
     </row>
-    <row r="462" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="462" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A462">
         <v>2019</v>
       </c>
@@ -12578,7 +12570,7 @@
       <c r="K462" s="4"/>
       <c r="L462" s="4"/>
     </row>
-    <row r="463" spans="1:12" ht="36" x14ac:dyDescent="0.25">
+    <row r="463" spans="1:12" ht="36" x14ac:dyDescent="0.3">
       <c r="A463">
         <v>2019</v>
       </c>
@@ -12602,7 +12594,7 @@
       <c r="K463" s="4"/>
       <c r="L463" s="4"/>
     </row>
-    <row r="464" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="464" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A464">
         <v>2019</v>
       </c>
@@ -12624,7 +12616,7 @@
       <c r="K464" s="4"/>
       <c r="L464" s="4"/>
     </row>
-    <row r="465" spans="1:12" ht="36" x14ac:dyDescent="0.25">
+    <row r="465" spans="1:12" ht="36" x14ac:dyDescent="0.3">
       <c r="A465">
         <v>2019</v>
       </c>
@@ -12646,7 +12638,7 @@
       <c r="K465" s="4"/>
       <c r="L465" s="4"/>
     </row>
-    <row r="466" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="466" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A466">
         <v>2019</v>
       </c>
@@ -12670,7 +12662,7 @@
       <c r="K466" s="4"/>
       <c r="L466" s="4"/>
     </row>
-    <row r="467" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="467" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A467">
         <v>2019</v>
       </c>
@@ -12692,7 +12684,7 @@
       <c r="K467" s="4"/>
       <c r="L467" s="4"/>
     </row>
-    <row r="468" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="468" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A468">
         <v>2019</v>
       </c>
@@ -12714,7 +12706,7 @@
       <c r="K468" s="4"/>
       <c r="L468" s="4"/>
     </row>
-    <row r="469" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="469" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A469">
         <v>2020</v>
       </c>
@@ -12738,7 +12730,7 @@
       <c r="K469" s="4"/>
       <c r="L469" s="4"/>
     </row>
-    <row r="470" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="470" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A470">
         <v>2020</v>
       </c>
@@ -12762,7 +12754,7 @@
       <c r="K470" s="4"/>
       <c r="L470" s="4"/>
     </row>
-    <row r="471" spans="1:12" ht="36" x14ac:dyDescent="0.25">
+    <row r="471" spans="1:12" ht="36" x14ac:dyDescent="0.3">
       <c r="A471">
         <v>2020</v>
       </c>
@@ -12786,7 +12778,7 @@
       <c r="K471" s="4"/>
       <c r="L471" s="4"/>
     </row>
-    <row r="472" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="472" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A472">
         <v>2020</v>
       </c>
@@ -12810,7 +12802,7 @@
       <c r="K472" s="4"/>
       <c r="L472" s="4"/>
     </row>
-    <row r="473" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="473" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A473">
         <v>2020</v>
       </c>
@@ -12832,7 +12824,7 @@
       <c r="K473" s="4"/>
       <c r="L473" s="4"/>
     </row>
-    <row r="474" spans="1:12" ht="36" x14ac:dyDescent="0.25">
+    <row r="474" spans="1:12" ht="36" x14ac:dyDescent="0.3">
       <c r="A474">
         <v>2020</v>
       </c>
@@ -12854,7 +12846,7 @@
       <c r="K474" s="4"/>
       <c r="L474" s="4"/>
     </row>
-    <row r="475" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="475" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A475">
         <v>2020</v>
       </c>
@@ -12878,7 +12870,7 @@
       <c r="K475" s="4"/>
       <c r="L475" s="4"/>
     </row>
-    <row r="476" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="476" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A476">
         <v>2020</v>
       </c>
@@ -12900,7 +12892,7 @@
       <c r="K476" s="4"/>
       <c r="L476" s="4"/>
     </row>
-    <row r="477" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="477" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A477">
         <v>2020</v>
       </c>
@@ -12922,7 +12914,7 @@
       <c r="K477" s="4"/>
       <c r="L477" s="4"/>
     </row>
-    <row r="478" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="478" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A478">
         <v>2020</v>
       </c>
@@ -12946,7 +12938,7 @@
       <c r="K478" s="4"/>
       <c r="L478" s="4"/>
     </row>
-    <row r="479" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="479" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A479">
         <v>2020</v>
       </c>
@@ -12968,7 +12960,7 @@
       <c r="K479" s="4"/>
       <c r="L479" s="4"/>
     </row>
-    <row r="480" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="480" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A480">
         <v>2020</v>
       </c>
@@ -12992,7 +12984,7 @@
       <c r="K480" s="4"/>
       <c r="L480" s="4"/>
     </row>
-    <row r="481" spans="1:12" ht="36" x14ac:dyDescent="0.25">
+    <row r="481" spans="1:12" ht="36" x14ac:dyDescent="0.3">
       <c r="A481">
         <v>2020</v>
       </c>
@@ -13016,7 +13008,7 @@
       <c r="K481" s="4"/>
       <c r="L481" s="4"/>
     </row>
-    <row r="482" spans="1:12" ht="36" x14ac:dyDescent="0.25">
+    <row r="482" spans="1:12" ht="36" x14ac:dyDescent="0.3">
       <c r="A482">
         <v>2020</v>
       </c>
@@ -13040,7 +13032,7 @@
       <c r="K482" s="4"/>
       <c r="L482" s="4"/>
     </row>
-    <row r="483" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="483" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A483">
         <v>2020</v>
       </c>
@@ -13062,7 +13054,7 @@
       <c r="K483" s="4"/>
       <c r="L483" s="4"/>
     </row>
-    <row r="484" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="484" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A484">
         <v>2020</v>
       </c>
@@ -13084,7 +13076,7 @@
       <c r="K484" s="4"/>
       <c r="L484" s="4"/>
     </row>
-    <row r="485" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="485" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A485">
         <v>2020</v>
       </c>
@@ -13108,7 +13100,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="486" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="486" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A486">
         <v>2020</v>
       </c>
@@ -13132,7 +13124,7 @@
       </c>
       <c r="L486" s="4"/>
     </row>
-    <row r="487" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="487" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A487">
         <v>2020</v>
       </c>
@@ -13156,7 +13148,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="488" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="488" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A488">
         <v>2020</v>
       </c>
@@ -13178,7 +13170,7 @@
       <c r="K488" s="4"/>
       <c r="L488" s="4"/>
     </row>
-    <row r="489" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="489" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A489">
         <v>2020</v>
       </c>
@@ -13200,7 +13192,7 @@
       <c r="K489" s="4"/>
       <c r="L489" s="4"/>
     </row>
-    <row r="490" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="490" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A490">
         <v>2020</v>
       </c>
@@ -13224,7 +13216,7 @@
       <c r="K490" s="4"/>
       <c r="L490" s="4"/>
     </row>
-    <row r="491" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="491" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A491">
         <v>2020</v>
       </c>
@@ -13246,7 +13238,7 @@
       <c r="K491" s="4"/>
       <c r="L491" s="4"/>
     </row>
-    <row r="492" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="492" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A492">
         <v>2020</v>
       </c>
@@ -13268,7 +13260,7 @@
       <c r="K492" s="4"/>
       <c r="L492" s="4"/>
     </row>
-    <row r="493" spans="1:12" ht="36" x14ac:dyDescent="0.25">
+    <row r="493" spans="1:12" ht="36" x14ac:dyDescent="0.3">
       <c r="A493">
         <v>2020</v>
       </c>
@@ -13292,7 +13284,7 @@
       <c r="K493" s="4"/>
       <c r="L493" s="4"/>
     </row>
-    <row r="494" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="494" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A494">
         <v>2020</v>
       </c>
@@ -13314,7 +13306,7 @@
       <c r="K494" s="4"/>
       <c r="L494" s="4"/>
     </row>
-    <row r="495" spans="1:12" ht="36" x14ac:dyDescent="0.25">
+    <row r="495" spans="1:12" ht="36" x14ac:dyDescent="0.3">
       <c r="A495">
         <v>2020</v>
       </c>
@@ -13336,7 +13328,7 @@
       <c r="K495" s="4"/>
       <c r="L495" s="4"/>
     </row>
-    <row r="496" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="496" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A496">
         <v>2020</v>
       </c>
@@ -13360,7 +13352,7 @@
       <c r="K496" s="4"/>
       <c r="L496" s="4"/>
     </row>
-    <row r="497" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="497" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A497">
         <v>2020</v>
       </c>
@@ -13382,7 +13374,7 @@
       <c r="K497" s="4"/>
       <c r="L497" s="4"/>
     </row>
-    <row r="498" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="498" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A498">
         <v>2020</v>
       </c>
@@ -13404,7 +13396,7 @@
       <c r="K498" s="4"/>
       <c r="L498" s="4"/>
     </row>
-    <row r="499" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="499" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A499">
         <v>2021</v>
       </c>
@@ -13428,7 +13420,7 @@
       <c r="K499" s="4"/>
       <c r="L499" s="4"/>
     </row>
-    <row r="500" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="500" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A500">
         <v>2021</v>
       </c>
@@ -13452,7 +13444,7 @@
       <c r="K500" s="4"/>
       <c r="L500" s="4"/>
     </row>
-    <row r="501" spans="1:12" ht="36" x14ac:dyDescent="0.25">
+    <row r="501" spans="1:12" ht="36" x14ac:dyDescent="0.3">
       <c r="A501">
         <v>2021</v>
       </c>
@@ -13476,7 +13468,7 @@
       <c r="K501" s="4"/>
       <c r="L501" s="4"/>
     </row>
-    <row r="502" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="502" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A502">
         <v>2021</v>
       </c>
@@ -13498,7 +13490,7 @@
       <c r="K502" s="4"/>
       <c r="L502" s="4"/>
     </row>
-    <row r="503" spans="1:12" ht="36" x14ac:dyDescent="0.25">
+    <row r="503" spans="1:12" ht="36" x14ac:dyDescent="0.3">
       <c r="A503">
         <v>2021</v>
       </c>
@@ -13520,7 +13512,7 @@
       <c r="K503" s="4"/>
       <c r="L503" s="4"/>
     </row>
-    <row r="504" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="504" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A504">
         <v>2021</v>
       </c>
@@ -13542,7 +13534,7 @@
       <c r="K504" s="4"/>
       <c r="L504" s="4"/>
     </row>
-    <row r="505" spans="1:12" ht="36" x14ac:dyDescent="0.25">
+    <row r="505" spans="1:12" ht="36" x14ac:dyDescent="0.3">
       <c r="A505">
         <v>2021</v>
       </c>
@@ -13566,7 +13558,7 @@
       <c r="K505" s="4"/>
       <c r="L505" s="4"/>
     </row>
-    <row r="506" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="506" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A506">
         <v>2021</v>
       </c>
@@ -13590,7 +13582,7 @@
       <c r="K506" s="4"/>
       <c r="L506" s="4"/>
     </row>
-    <row r="507" spans="1:12" ht="36" x14ac:dyDescent="0.25">
+    <row r="507" spans="1:12" ht="36" x14ac:dyDescent="0.3">
       <c r="A507">
         <v>2021</v>
       </c>
@@ -13612,7 +13604,7 @@
       <c r="K507" s="4"/>
       <c r="L507" s="4"/>
     </row>
-    <row r="508" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="508" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A508">
         <v>2021</v>
       </c>
@@ -13636,7 +13628,7 @@
       <c r="K508" s="4"/>
       <c r="L508" s="4"/>
     </row>
-    <row r="509" spans="1:12" ht="36" x14ac:dyDescent="0.25">
+    <row r="509" spans="1:12" ht="36" x14ac:dyDescent="0.3">
       <c r="A509">
         <v>2021</v>
       </c>
@@ -13660,7 +13652,7 @@
       <c r="K509" s="4"/>
       <c r="L509" s="4"/>
     </row>
-    <row r="510" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="510" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A510">
         <v>2021</v>
       </c>
@@ -13684,7 +13676,7 @@
       <c r="K510" s="4"/>
       <c r="L510" s="4"/>
     </row>
-    <row r="511" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="511" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A511">
         <v>2021</v>
       </c>
@@ -13708,7 +13700,7 @@
       <c r="K511" s="4"/>
       <c r="L511" s="4"/>
     </row>
-    <row r="512" spans="1:12" ht="36" x14ac:dyDescent="0.25">
+    <row r="512" spans="1:12" ht="36" x14ac:dyDescent="0.3">
       <c r="A512">
         <v>2021</v>
       </c>
@@ -13730,7 +13722,7 @@
       <c r="K512" s="4"/>
       <c r="L512" s="4"/>
     </row>
-    <row r="513" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="513" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A513">
         <v>2021</v>
       </c>
@@ -13752,7 +13744,7 @@
       <c r="K513" s="4"/>
       <c r="L513" s="4"/>
     </row>
-    <row r="514" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="514" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A514">
         <v>2021</v>
       </c>
@@ -13774,7 +13766,7 @@
       <c r="K514" s="4"/>
       <c r="L514" s="4"/>
     </row>
-    <row r="515" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="515" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A515">
         <v>2021</v>
       </c>
@@ -13798,7 +13790,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="516" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="516" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A516">
         <v>2021</v>
       </c>
@@ -13822,7 +13814,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="517" spans="1:12" ht="36" x14ac:dyDescent="0.25">
+    <row r="517" spans="1:12" ht="36" x14ac:dyDescent="0.3">
       <c r="A517">
         <v>2021</v>
       </c>
@@ -13846,7 +13838,7 @@
       </c>
       <c r="L517" s="4"/>
     </row>
-    <row r="518" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="518" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A518">
         <v>2021</v>
       </c>
@@ -13868,7 +13860,7 @@
       <c r="K518" s="4"/>
       <c r="L518" s="4"/>
     </row>
-    <row r="519" spans="1:12" ht="36" x14ac:dyDescent="0.25">
+    <row r="519" spans="1:12" ht="36" x14ac:dyDescent="0.3">
       <c r="A519">
         <v>2021</v>
       </c>
@@ -13890,7 +13882,7 @@
       <c r="K519" s="4"/>
       <c r="L519" s="4"/>
     </row>
-    <row r="520" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="520" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A520">
         <v>2021</v>
       </c>
@@ -13912,7 +13904,7 @@
       <c r="K520" s="4"/>
       <c r="L520" s="4"/>
     </row>
-    <row r="521" spans="1:12" ht="36" x14ac:dyDescent="0.25">
+    <row r="521" spans="1:12" ht="36" x14ac:dyDescent="0.3">
       <c r="A521">
         <v>2021</v>
       </c>
@@ -13934,7 +13926,7 @@
       <c r="K521" s="4"/>
       <c r="L521" s="4"/>
     </row>
-    <row r="522" spans="1:12" ht="36" x14ac:dyDescent="0.25">
+    <row r="522" spans="1:12" ht="36" x14ac:dyDescent="0.3">
       <c r="A522">
         <v>2021</v>
       </c>
@@ -13958,7 +13950,7 @@
       <c r="K522" s="4"/>
       <c r="L522" s="4"/>
     </row>
-    <row r="523" spans="1:12" ht="36" x14ac:dyDescent="0.25">
+    <row r="523" spans="1:12" ht="36" x14ac:dyDescent="0.3">
       <c r="A523">
         <v>2021</v>
       </c>
@@ -13982,7 +13974,7 @@
       <c r="K523" s="4"/>
       <c r="L523" s="4"/>
     </row>
-    <row r="524" spans="1:12" ht="24" x14ac:dyDescent="0.25">
+    <row r="524" spans="1:12" ht="24" x14ac:dyDescent="0.3">
       <c r="A524">
         <v>2021</v>
       </c>
@@ -14004,7 +13996,7 @@
       <c r="K524" s="4"/>
       <c r="L524" s="4"/>
     </row>
-    <row r="525" spans="1:12" ht="36" x14ac:dyDescent="0.25">
+    <row r="525" spans="1:12" ht="36" x14ac:dyDescent="0.3">
       <c r="A525">
         <v>2021</v>
       </c>
@@ -14026,7 +14018,7 @@
       <c r="K525" s="4"/>
       <c r="L525" s="4"/>
     </row>
-    <row r="526" spans="1:12" ht="36" x14ac:dyDescent="0.25">
+    <row r="526" spans="1:12" ht="36" x14ac:dyDescent="0.3">
       <c r="A526">
         <v>2021</v>
       </c>
@@ -14048,7 +14040,7 @@
       <c r="K526" s="4"/>
       <c r="L526" s="4"/>
     </row>
-    <row r="527" spans="1:12" ht="36" x14ac:dyDescent="0.25">
+    <row r="527" spans="1:12" ht="36" x14ac:dyDescent="0.3">
       <c r="A527">
         <v>2021</v>
       </c>
@@ -14070,7 +14062,7 @@
       <c r="K527" s="4"/>
       <c r="L527" s="4"/>
     </row>
-    <row r="528" spans="1:12" ht="36" x14ac:dyDescent="0.25">
+    <row r="528" spans="1:12" ht="36" x14ac:dyDescent="0.3">
       <c r="A528">
         <v>2021</v>
       </c>
@@ -14092,7 +14084,7 @@
       <c r="K528" s="4"/>
       <c r="L528" s="4"/>
     </row>
-    <row r="529" spans="1:12" ht="36" x14ac:dyDescent="0.25">
+    <row r="529" spans="1:12" ht="36" x14ac:dyDescent="0.3">
       <c r="A529">
         <v>2021</v>
       </c>
@@ -14116,7 +14108,7 @@
       <c r="K529" s="4"/>
       <c r="L529" s="4"/>
     </row>
-    <row r="530" spans="1:12" ht="36" x14ac:dyDescent="0.25">
+    <row r="530" spans="1:12" ht="36" x14ac:dyDescent="0.3">
       <c r="A530">
         <v>2021</v>
       </c>
@@ -14138,7 +14130,7 @@
       <c r="K530" s="4"/>
       <c r="L530" s="4"/>
     </row>
-    <row r="531" spans="1:12" ht="36" x14ac:dyDescent="0.25">
+    <row r="531" spans="1:12" ht="36" x14ac:dyDescent="0.3">
       <c r="A531">
         <v>2021</v>
       </c>
@@ -14160,7 +14152,7 @@
       <c r="K531" s="4"/>
       <c r="L531" s="4"/>
     </row>
-    <row r="532" spans="1:12" ht="36" x14ac:dyDescent="0.25">
+    <row r="532" spans="1:12" ht="36" x14ac:dyDescent="0.3">
       <c r="A532">
         <v>2021</v>
       </c>
@@ -14182,7 +14174,7 @@
       <c r="K532" s="4"/>
       <c r="L532" s="4"/>
     </row>
-    <row r="533" spans="1:12" ht="36" x14ac:dyDescent="0.25">
+    <row r="533" spans="1:12" ht="36" x14ac:dyDescent="0.3">
       <c r="A533">
         <v>2021</v>
       </c>

</xml_diff>